<commit_message>
Done enhancement, SKU validation not yet
</commit_message>
<xml_diff>
--- a/files/temporaryTemplates/TempOrderHoneywell.xlsx
+++ b/files/temporaryTemplates/TempOrderHoneywell.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Reports\ConversionToolExcelToExcel\temporaryTemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Reports\conversionToolBack\files\temporaryTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A12307-9B37-4B4A-B75A-6C3E8E340470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB4B36F1-C7D8-4395-A7A4-2693B99546E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,8 +19,144 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>FLUX</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Date FormatYYYY-MM-DD</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Date FormatYYYY-MM-DD</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Date FormatYYYY-MM-DD</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Date FormatYYYY-MM-DD</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DL1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Date FormatYYYY-MM-DD</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DM1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Date FormatYYYY-MM-DD</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DN1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Date FormatYYYY-MM-DD</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EH1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Date FormatYYYY-MM-DD</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EK1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Date FormatYYYY-MM-DD</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="566">
   <si>
     <t>Warehouse ID</t>
   </si>
@@ -304,13 +440,13 @@
     <t>billingFax</t>
   </si>
   <si>
-    <t>Billing TEL1</t>
+    <t>Billing Telphone1</t>
   </si>
   <si>
     <t>billingTel1</t>
   </si>
   <si>
-    <t>Billing TEL2</t>
+    <t>Billing Telphone2</t>
   </si>
   <si>
     <t>billingTel2</t>
@@ -472,18 +608,21 @@
     <t>carrierFax</t>
   </si>
   <si>
-    <t>Carrier TEL1</t>
+    <t>Carrier Telphone1</t>
   </si>
   <si>
     <t>carrierTel1</t>
   </si>
   <si>
-    <t>Carrier TEL2</t>
+    <t>Carrier Telphone2</t>
   </si>
   <si>
     <t>carrierTel2</t>
   </si>
   <si>
+    <t>Issue Party ID</t>
+  </si>
+  <si>
     <t>issuePartyId</t>
   </si>
   <si>
@@ -571,13 +710,13 @@
     <t>issuePartyFax</t>
   </si>
   <si>
-    <t>Issue Party TEL1</t>
+    <t>Issue Party Telphone1</t>
   </si>
   <si>
     <t>issuePartyTel1</t>
   </si>
   <si>
-    <t>Issue Party TEL2</t>
+    <t>Issue Party Telphone2</t>
   </si>
   <si>
     <t>issuePartyTel2</t>
@@ -781,318 +920,312 @@
     <t>rfGetTask</t>
   </si>
   <si>
-    <t>ERP Cancel Flag</t>
+    <t>Single Match</t>
+  </si>
+  <si>
+    <t>singleMatch</t>
+  </si>
+  <si>
+    <t>SerialNO Catch</t>
+  </si>
+  <si>
+    <t>serialNoCatch</t>
+  </si>
+  <si>
+    <t>Require DeliveryNO</t>
+  </si>
+  <si>
+    <t>requireDeliveryNo</t>
+  </si>
+  <si>
+    <t>Archive Flag</t>
+  </si>
+  <si>
+    <t>archiveFlag</t>
+  </si>
+  <si>
+    <t>Allow Partial Allocation</t>
+  </si>
+  <si>
+    <t>ful_alc</t>
+  </si>
+  <si>
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>channel</t>
+  </si>
+  <si>
+    <t>Weighting Flag</t>
+  </si>
+  <si>
+    <t>weightingFlag</t>
+  </si>
+  <si>
+    <t>Allow Shipment</t>
+  </si>
+  <si>
+    <t>allowShipment</t>
+  </si>
+  <si>
+    <t>Allow Partial Ship</t>
+  </si>
+  <si>
+    <t>allowPartialShip</t>
+  </si>
+  <si>
+    <t>EDI Carrier Flag</t>
+  </si>
+  <si>
+    <t>ediCarrierFlag</t>
+  </si>
+  <si>
+    <t>Last Shipment Time</t>
+  </si>
+  <si>
+    <t>lastShipmentTime</t>
+  </si>
+  <si>
+    <t>Create Source</t>
+  </si>
+  <si>
+    <t>createSource</t>
+  </si>
+  <si>
+    <t>Zone Group</t>
+  </si>
+  <si>
+    <t>zoneGroup</t>
+  </si>
+  <si>
+    <t>Medical Xml Time</t>
+  </si>
+  <si>
+    <t>medicalXmlTime</t>
+  </si>
+  <si>
+    <t>Follow Up</t>
+  </si>
+  <si>
+    <t>followUp</t>
+  </si>
+  <si>
+    <t>Sales Orderno</t>
+  </si>
+  <si>
+    <t>salesOrderNo</t>
+  </si>
+  <si>
+    <t>Put Location TO</t>
+  </si>
+  <si>
+    <t>putToLocation</t>
+  </si>
+  <si>
+    <t>DeliveryNO</t>
+  </si>
+  <si>
+    <t>deliveryNo</t>
+  </si>
+  <si>
+    <t>Allocation Count</t>
+  </si>
+  <si>
+    <t>allocationCount</t>
+  </si>
+  <si>
+    <t>WaveNO</t>
+  </si>
+  <si>
+    <t>waveNo</t>
+  </si>
+  <si>
+    <t>Carton Group</t>
+  </si>
+  <si>
+    <t>cartonGroup</t>
+  </si>
+  <si>
+    <t>Carton ID</t>
+  </si>
+  <si>
+    <t>cartonId</t>
+  </si>
+  <si>
+    <t>Order GroupNO</t>
+  </si>
+  <si>
+    <t>orderGroupNo</t>
+  </si>
+  <si>
+    <t>Trans Service Level</t>
+  </si>
+  <si>
+    <t>transServiceLevel</t>
+  </si>
+  <si>
+    <t>Order Handle Instruction</t>
+  </si>
+  <si>
+    <t>orderHandleInstruction</t>
+  </si>
+  <si>
+    <t>Total Cubic</t>
+  </si>
+  <si>
+    <t>totalCubic</t>
+  </si>
+  <si>
+    <t>Total Gross Weight</t>
+  </si>
+  <si>
+    <t>totalGrossWeight</t>
+  </si>
+  <si>
+    <t>Total Net Weight</t>
+  </si>
+  <si>
+    <t>totalNetWeight</t>
+  </si>
+  <si>
+    <t>Total Price</t>
+  </si>
+  <si>
+    <t>totalPrice</t>
+  </si>
+  <si>
+    <t>Total Line Count</t>
+  </si>
+  <si>
+    <t>totalLineCount</t>
+  </si>
+  <si>
+    <t>Cur LineNO</t>
+  </si>
+  <si>
+    <t>curLineNo</t>
+  </si>
+  <si>
+    <t>Parcel Mark</t>
+  </si>
+  <si>
+    <t>parcelMark</t>
+  </si>
+  <si>
+    <t>Parcel Consolidation</t>
+  </si>
+  <si>
+    <t>parcelConsolidation</t>
+  </si>
+  <si>
+    <t>Total SKU Count</t>
+  </si>
+  <si>
+    <t>totalSkuCount</t>
+  </si>
+  <si>
+    <t>Warehouse Transfer Flag</t>
+  </si>
+  <si>
+    <t>warehouseTransferFlag</t>
+  </si>
+  <si>
+    <t>Express Platform</t>
+  </si>
+  <si>
+    <t>expressPlatform</t>
+  </si>
+  <si>
+    <t>OCP NO</t>
+  </si>
+  <si>
+    <t>ocpNo</t>
+  </si>
+  <si>
+    <t>VehicleNO</t>
+  </si>
+  <si>
+    <t>vehicleNo</t>
+  </si>
+  <si>
+    <t>Vehicle Type</t>
+  </si>
+  <si>
+    <t>vehicleType</t>
+  </si>
+  <si>
+    <t>Driver</t>
+  </si>
+  <si>
+    <t>driver</t>
+  </si>
+  <si>
+    <t>Split Flag</t>
+  </si>
+  <si>
+    <t>splitFlag</t>
+  </si>
+  <si>
+    <t>Loc Group1 List</t>
+  </si>
+  <si>
+    <t>locGroup1List</t>
+  </si>
+  <si>
+    <t>Loc Group2 List</t>
+  </si>
+  <si>
+    <t>locGroup2List</t>
+  </si>
+  <si>
+    <t>Shipment Count</t>
+  </si>
+  <si>
+    <t>shipmentCount</t>
+  </si>
+  <si>
+    <t>Wave Rule</t>
+  </si>
+  <si>
+    <t>waveRule</t>
+  </si>
+  <si>
+    <t>Reverse Order NO</t>
+  </si>
+  <si>
+    <t>reverseOrderNo</t>
+  </si>
+  <si>
+    <t>Shop</t>
+  </si>
+  <si>
+    <t>shop</t>
+  </si>
+  <si>
+    <t>Replenish Group ID</t>
+  </si>
+  <si>
+    <t>rpGroupId</t>
+  </si>
+  <si>
+    <t>Total QTY</t>
+  </si>
+  <si>
+    <t>totalQty</t>
+  </si>
+  <si>
+    <t>Crossdock Flag</t>
+  </si>
+  <si>
+    <t>crossdockFlag</t>
+  </si>
+  <si>
+    <t>Erp Cancel Flag</t>
   </si>
   <si>
     <t>erpCancelFlag</t>
   </si>
   <si>
-    <t>Single Match</t>
-  </si>
-  <si>
-    <t>singleMatch</t>
-  </si>
-  <si>
-    <t>SerialNO Catch</t>
-  </si>
-  <si>
-    <t>serialNoCatch</t>
-  </si>
-  <si>
-    <t>Require DeliveryNO</t>
-  </si>
-  <si>
-    <t>requireDeliveryNo</t>
-  </si>
-  <si>
-    <t>Archive Flag</t>
-  </si>
-  <si>
-    <t>archiveFlag</t>
-  </si>
-  <si>
-    <t>FUL ALC</t>
-  </si>
-  <si>
-    <t>ful_alc</t>
-  </si>
-  <si>
-    <t>Channel</t>
-  </si>
-  <si>
-    <t>channel</t>
-  </si>
-  <si>
-    <t>Weighting Flag</t>
-  </si>
-  <si>
-    <t>weightingFlag</t>
-  </si>
-  <si>
-    <t>Allow Shipment</t>
-  </si>
-  <si>
-    <t>allowShipment</t>
-  </si>
-  <si>
-    <t>Allow Partial Ship</t>
-  </si>
-  <si>
-    <t>allowPartialShip</t>
-  </si>
-  <si>
-    <t>EDI Carrier Flag</t>
-  </si>
-  <si>
-    <t>ediCarrierFlag</t>
-  </si>
-  <si>
-    <t>Last Shipment Time</t>
-  </si>
-  <si>
-    <t>lastShipmentTime</t>
-  </si>
-  <si>
-    <t>Create Source</t>
-  </si>
-  <si>
-    <t>createSource</t>
-  </si>
-  <si>
-    <t>Zone Group</t>
-  </si>
-  <si>
-    <t>zoneGroup</t>
-  </si>
-  <si>
-    <t>Medical Xml Time</t>
-  </si>
-  <si>
-    <t>medicalXmlTime</t>
-  </si>
-  <si>
-    <t>Follow Up</t>
-  </si>
-  <si>
-    <t>followUp</t>
-  </si>
-  <si>
-    <t>Sales Orderno</t>
-  </si>
-  <si>
-    <t>salesOrderno</t>
-  </si>
-  <si>
-    <t>Put Location TO</t>
-  </si>
-  <si>
-    <t>putToLocation</t>
-  </si>
-  <si>
-    <t>DeliveryNO</t>
-  </si>
-  <si>
-    <t>deliveryNo</t>
-  </si>
-  <si>
-    <t>Allocation Count</t>
-  </si>
-  <si>
-    <t>allocationCount</t>
-  </si>
-  <si>
-    <t>WaveNO</t>
-  </si>
-  <si>
-    <t>waveNo</t>
-  </si>
-  <si>
-    <t>Carton Group</t>
-  </si>
-  <si>
-    <t>cartonGroup</t>
-  </si>
-  <si>
-    <t>Carton ID</t>
-  </si>
-  <si>
-    <t>cartonId</t>
-  </si>
-  <si>
-    <t>Order GroupNO</t>
-  </si>
-  <si>
-    <t>orderGroupNo</t>
-  </si>
-  <si>
-    <t>Trans Service Level</t>
-  </si>
-  <si>
-    <t>transServiceLevel</t>
-  </si>
-  <si>
-    <t>Order Handle Instruction</t>
-  </si>
-  <si>
-    <t>orderHandleInstruction</t>
-  </si>
-  <si>
-    <t>Total Cubic</t>
-  </si>
-  <si>
-    <t>totalCubic</t>
-  </si>
-  <si>
-    <t>Total Gross Weight</t>
-  </si>
-  <si>
-    <t>totalGrossWeight</t>
-  </si>
-  <si>
-    <t>Total Net Weight</t>
-  </si>
-  <si>
-    <t>totalNetWeight</t>
-  </si>
-  <si>
-    <t>Total Price</t>
-  </si>
-  <si>
-    <t>totalPrice</t>
-  </si>
-  <si>
-    <t>Total Line Count</t>
-  </si>
-  <si>
-    <t>totalLineCount</t>
-  </si>
-  <si>
-    <t>Cur LineNO</t>
-  </si>
-  <si>
-    <t>curLineNo</t>
-  </si>
-  <si>
-    <t>Parcel Mark</t>
-  </si>
-  <si>
-    <t>parcelMark</t>
-  </si>
-  <si>
-    <t>Parcel Consolidation</t>
-  </si>
-  <si>
-    <t>parcelConsolidation</t>
-  </si>
-  <si>
-    <t>Total SKU Count</t>
-  </si>
-  <si>
-    <t>totalSkuCount</t>
-  </si>
-  <si>
-    <t>Warehouse Transfer Flag</t>
-  </si>
-  <si>
-    <t>warehouseTransferFlag</t>
-  </si>
-  <si>
-    <t>ERP Cancel Reason</t>
-  </si>
-  <si>
-    <t>erpCancelReason</t>
-  </si>
-  <si>
-    <t>Express Platform</t>
-  </si>
-  <si>
-    <t>expressPlatform</t>
-  </si>
-  <si>
-    <t>OCP NO</t>
-  </si>
-  <si>
-    <t>ocpNo</t>
-  </si>
-  <si>
-    <t>VehicleNO</t>
-  </si>
-  <si>
-    <t>vehicleNo</t>
-  </si>
-  <si>
-    <t>Vehicle Type</t>
-  </si>
-  <si>
-    <t>vehicleType</t>
-  </si>
-  <si>
-    <t>Driver</t>
-  </si>
-  <si>
-    <t>driver</t>
-  </si>
-  <si>
-    <t>Split Flag</t>
-  </si>
-  <si>
-    <t>splitFlag</t>
-  </si>
-  <si>
-    <t>Order Source</t>
-  </si>
-  <si>
-    <t>orderSource</t>
-  </si>
-  <si>
-    <t>LOC Group1 List</t>
-  </si>
-  <si>
-    <t>locGroup1List</t>
-  </si>
-  <si>
-    <t>LOC Group2 List</t>
-  </si>
-  <si>
-    <t>locGroup2List</t>
-  </si>
-  <si>
-    <t>Shipment Count</t>
-  </si>
-  <si>
-    <t>shipmentCount</t>
-  </si>
-  <si>
-    <t>Wave Rule</t>
-  </si>
-  <si>
-    <t>waveRule</t>
-  </si>
-  <si>
-    <t>Reverse Order NO</t>
-  </si>
-  <si>
-    <t>reverseOrderno</t>
-  </si>
-  <si>
-    <t>Shop</t>
-  </si>
-  <si>
-    <t>shop</t>
-  </si>
-  <si>
-    <t>Replenish Group ID</t>
-  </si>
-  <si>
-    <t>rpGroupId</t>
-  </si>
-  <si>
-    <t>Total QTY</t>
-  </si>
-  <si>
-    <t>totalQty</t>
-  </si>
-  <si>
     <t>Note Text</t>
   </si>
   <si>
@@ -1135,6 +1268,12 @@
     <t>udf06</t>
   </si>
   <si>
+    <t>Task Flag</t>
+  </si>
+  <si>
+    <t>taskFlag</t>
+  </si>
+  <si>
     <t>D.warehouseId</t>
   </si>
   <si>
@@ -1369,55 +1508,55 @@
     <t>D.price</t>
   </si>
   <si>
-    <t>DEDI01</t>
+    <t>DEDI1</t>
   </si>
   <si>
     <t>D.dedi01</t>
   </si>
   <si>
-    <t>DEDI02</t>
+    <t>DEDI2</t>
   </si>
   <si>
     <t>D.dedi02</t>
   </si>
   <si>
-    <t>DEDI03</t>
+    <t>DEDI3</t>
   </si>
   <si>
     <t>D.dedi03</t>
   </si>
   <si>
-    <t>DEDI04</t>
+    <t>DEDI4</t>
   </si>
   <si>
     <t>D.dedi04</t>
   </si>
   <si>
-    <t>DEDI05</t>
+    <t>DEDI5</t>
   </si>
   <si>
     <t>D.dedi05</t>
   </si>
   <si>
-    <t>DEDI06</t>
+    <t>DEDI6</t>
   </si>
   <si>
     <t>D.dedi06</t>
   </si>
   <si>
-    <t>DEDI07</t>
+    <t>DEDI7</t>
   </si>
   <si>
     <t>D.dedi07</t>
   </si>
   <si>
-    <t>DEDI08</t>
+    <t>DEDI8</t>
   </si>
   <si>
     <t>D.dedi08</t>
   </si>
   <si>
-    <t>DEDI09</t>
+    <t>DEDI9</t>
   </si>
   <si>
     <t>D.dedi09</t>
@@ -1489,259 +1628,232 @@
     <t>D.dedi20</t>
   </si>
   <si>
+    <t>原產品名</t>
+  </si>
+  <si>
+    <t>D.originalSku</t>
+  </si>
+  <si>
+    <t>Kit ReferenceNO</t>
+  </si>
+  <si>
+    <t>D.kitReferenceNo</t>
+  </si>
+  <si>
+    <t>Order Line ReferenceNO</t>
+  </si>
+  <si>
+    <t>D.orderLineReferenceNo</t>
+  </si>
+  <si>
+    <t>Kit SKU</t>
+  </si>
+  <si>
+    <t>D.kitSku</t>
+  </si>
+  <si>
+    <t>D.erpCancelFlag</t>
+  </si>
+  <si>
+    <t>D.zoneGroup</t>
+  </si>
+  <si>
+    <t>LOC Group1</t>
+  </si>
+  <si>
+    <t>D.locGroup1</t>
+  </si>
+  <si>
+    <t>LOC Group2</t>
+  </si>
+  <si>
+    <t>D.locGroup2</t>
+  </si>
+  <si>
+    <t>Commingle SKU</t>
+  </si>
+  <si>
+    <t>D.commingleSku</t>
+  </si>
+  <si>
+    <t>One Step Allocation</t>
+  </si>
+  <si>
+    <t>D.oneStepAllocation</t>
+  </si>
+  <si>
+    <t>Order LOT Control</t>
+  </si>
+  <si>
+    <t>D.orderLotControl</t>
+  </si>
+  <si>
+    <t>Full Case LOT Control</t>
+  </si>
+  <si>
+    <t>D.fullCaseLotControl</t>
+  </si>
+  <si>
+    <t>Piece LOT Control</t>
+  </si>
+  <si>
+    <t>D.pieceLotControl</t>
+  </si>
+  <si>
+    <t>Reference LineNO</t>
+  </si>
+  <si>
+    <t>D.referenceLineNo</t>
+  </si>
+  <si>
+    <t>D.salesOrderNo</t>
+  </si>
+  <si>
+    <t>Sales Order LineNO</t>
+  </si>
+  <si>
+    <t>D.salesOrderLineNo</t>
+  </si>
+  <si>
+    <t>QTY Released</t>
+  </si>
+  <si>
+    <t>D.qtyReleased</t>
+  </si>
+  <si>
+    <t>Free Pick Gift</t>
+  </si>
+  <si>
+    <t>D.freePickGift</t>
+  </si>
+  <si>
+    <t>Rule3 Flag</t>
+  </si>
+  <si>
+    <t>D.rule3Flag</t>
+  </si>
+  <si>
+    <t>Allocation Where Sql</t>
+  </si>
+  <si>
+    <t>D.allocationWhereSql</t>
+  </si>
+  <si>
+    <t>D.noteText</t>
+  </si>
+  <si>
+    <t>D.udf01</t>
+  </si>
+  <si>
+    <t>D.udf02</t>
+  </si>
+  <si>
+    <t>D.udf03</t>
+  </si>
+  <si>
+    <t>D.udf04</t>
+  </si>
+  <si>
+    <t>D.udf05</t>
+  </si>
+  <si>
+    <t>D.udf06</t>
+  </si>
+  <si>
+    <t>LOTATT13</t>
+  </si>
+  <si>
+    <t>D.lotAtt13</t>
+  </si>
+  <si>
+    <t>LOTATT14</t>
+  </si>
+  <si>
+    <t>D.lotAtt14</t>
+  </si>
+  <si>
+    <t>LOTATT15</t>
+  </si>
+  <si>
+    <t>D.lotAtt15</t>
+  </si>
+  <si>
+    <t>LOTATT16</t>
+  </si>
+  <si>
+    <t>D.lotAtt16</t>
+  </si>
+  <si>
+    <t>LOTATT17</t>
+  </si>
+  <si>
+    <t>D.lotAtt17</t>
+  </si>
+  <si>
+    <t>LOTATT18</t>
+  </si>
+  <si>
+    <t>D.lotAtt18</t>
+  </si>
+  <si>
+    <t>LOTATT19</t>
+  </si>
+  <si>
+    <t>D.lotAtt19</t>
+  </si>
+  <si>
+    <t>LOTATT20</t>
+  </si>
+  <si>
+    <t>D.lotAtt20</t>
+  </si>
+  <si>
+    <t>LOTATT21</t>
+  </si>
+  <si>
+    <t>D.lotAtt21</t>
+  </si>
+  <si>
+    <t>LOTATT22</t>
+  </si>
+  <si>
+    <t>D.lotAtt22</t>
+  </si>
+  <si>
+    <t>LOTATT23</t>
+  </si>
+  <si>
+    <t>D.lotAtt23</t>
+  </si>
+  <si>
+    <t>LOTATT24</t>
+  </si>
+  <si>
+    <t>D.lotAtt24</t>
+  </si>
+  <si>
+    <t>MUID</t>
+  </si>
+  <si>
+    <t>D.muid</t>
+  </si>
+  <si>
+    <t>Pick Instruction</t>
+  </si>
+  <si>
+    <t>D.pickInstruction</t>
+  </si>
+  <si>
     <t>Alternative SKU</t>
   </si>
   <si>
     <t>D.alternativeSku</t>
   </si>
   <si>
-    <t>Kit ReferenceNO</t>
-  </si>
-  <si>
-    <t>D.kitReferenceNo</t>
-  </si>
-  <si>
-    <t>Order Line ReferenceNO</t>
-  </si>
-  <si>
-    <t>D.orderLineReferenceNo</t>
-  </si>
-  <si>
-    <t>Kit SKU</t>
-  </si>
-  <si>
-    <t>D.kitSku</t>
-  </si>
-  <si>
-    <t>D.erpCancelFlag</t>
-  </si>
-  <si>
-    <t>D.zoneGroup</t>
-  </si>
-  <si>
-    <t>LOC Group1</t>
-  </si>
-  <si>
-    <t>D.locGroup1</t>
-  </si>
-  <si>
-    <t>LOC Group2</t>
-  </si>
-  <si>
-    <t>D.locGroup2</t>
-  </si>
-  <si>
-    <t>Commingle SKU</t>
-  </si>
-  <si>
-    <t>D.commingleSku</t>
-  </si>
-  <si>
-    <t>One Step Allocation</t>
-  </si>
-  <si>
-    <t>D.oneStepAllocation</t>
-  </si>
-  <si>
-    <t>Order LOT Control</t>
-  </si>
-  <si>
-    <t>D.orderLotControl</t>
-  </si>
-  <si>
-    <t>Full Case LOT Control</t>
-  </si>
-  <si>
-    <t>D.fullCaseLotControl</t>
-  </si>
-  <si>
-    <t>Piece LOT Control</t>
-  </si>
-  <si>
-    <t>D.pieceLotControl</t>
-  </si>
-  <si>
-    <t>Reference LineNO</t>
-  </si>
-  <si>
-    <t>D.referenceLineNo</t>
-  </si>
-  <si>
-    <t>D.salesOrderNo</t>
-  </si>
-  <si>
-    <t>Sales Order LineNO</t>
-  </si>
-  <si>
-    <t>D.salesOrderLineNo</t>
-  </si>
-  <si>
-    <t>QTY Released</t>
-  </si>
-  <si>
-    <t>D.qtyReleased</t>
-  </si>
-  <si>
-    <t>Free Pick Gift</t>
-  </si>
-  <si>
-    <t>D.freePickGift</t>
-  </si>
-  <si>
-    <t>Rule3 Flag</t>
-  </si>
-  <si>
-    <t>D.rule3Flag</t>
-  </si>
-  <si>
-    <t>Allocation Where Sql</t>
-  </si>
-  <si>
-    <t>D.allocationWhereSql</t>
-  </si>
-  <si>
-    <t>D.noteText</t>
-  </si>
-  <si>
-    <t>D.udf01</t>
-  </si>
-  <si>
-    <t>D.udf02</t>
-  </si>
-  <si>
-    <t>D.udf03</t>
-  </si>
-  <si>
-    <t>D.udf04</t>
-  </si>
-  <si>
-    <t>D.udf05</t>
-  </si>
-  <si>
-    <t>D.udf06</t>
-  </si>
-  <si>
-    <t>LOTATT13</t>
-  </si>
-  <si>
-    <t>D.lotAtt13</t>
-  </si>
-  <si>
-    <t>LOTATT14</t>
-  </si>
-  <si>
-    <t>D.lotAtt14</t>
-  </si>
-  <si>
-    <t>LOTATT15</t>
-  </si>
-  <si>
-    <t>D.lotAtt15</t>
-  </si>
-  <si>
-    <t>LOTATT16</t>
-  </si>
-  <si>
-    <t>D.lotAtt16</t>
-  </si>
-  <si>
-    <t>LOTATT17</t>
-  </si>
-  <si>
-    <t>D.lotAtt17</t>
-  </si>
-  <si>
-    <t>LOTATT18</t>
-  </si>
-  <si>
-    <t>D.lotAtt18</t>
-  </si>
-  <si>
-    <t>LOTATT19</t>
-  </si>
-  <si>
-    <t>D.lotAtt19</t>
-  </si>
-  <si>
-    <t>LOTATT20</t>
-  </si>
-  <si>
-    <t>D.lotAtt20</t>
-  </si>
-  <si>
-    <t>LOTATT21</t>
-  </si>
-  <si>
-    <t>D.lotAtt21</t>
-  </si>
-  <si>
-    <t>LOTATT22</t>
-  </si>
-  <si>
-    <t>D.lotAtt22</t>
-  </si>
-  <si>
-    <t>LOTATT23</t>
-  </si>
-  <si>
-    <t>D.lotAtt23</t>
-  </si>
-  <si>
-    <t>LOTATT24</t>
-  </si>
-  <si>
-    <t>D.lotAtt24</t>
-  </si>
-  <si>
-    <t>MUID</t>
-  </si>
-  <si>
-    <t>D.muid</t>
-  </si>
-  <si>
-    <t>Pick Instruction</t>
-  </si>
-  <si>
-    <t>D.pickInstruction</t>
-  </si>
-  <si>
-    <t>Ship to</t>
-  </si>
-  <si>
-    <t>Warehouse ID Item</t>
-  </si>
-  <si>
-    <t>Customer ID Item</t>
-  </si>
-  <si>
-    <t>Erp Cancel Flag Item</t>
-  </si>
-  <si>
-    <t>Zone Group Item</t>
-  </si>
-  <si>
-    <t>Sales OrderNO Item</t>
-  </si>
-  <si>
-    <t>Note Text Item</t>
-  </si>
-  <si>
-    <t>UDF01 Item</t>
-  </si>
-  <si>
-    <t>UDF02 Item</t>
-  </si>
-  <si>
-    <t>UDF03 Item</t>
-  </si>
-  <si>
-    <t>UDF04 Item</t>
-  </si>
-  <si>
-    <t>UDF05 Item</t>
-  </si>
-  <si>
-    <t>UDF06 Item</t>
+    <t>Reference Line No</t>
+  </si>
+  <si>
+    <t>D.refLineNo</t>
   </si>
 </sst>
 </file>
@@ -1796,7 +1908,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="290">
+  <cellXfs count="292">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1941,7 +2053,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1975,14 +2086,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2067,6 +2179,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2404,306 +2518,308 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:KA2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:KC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="JA1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="JG8" sqref="JG8"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.140625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14" style="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.28515625" style="25" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.28515625" style="26" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.7109375" style="27" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18" style="28" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.7109375" style="30" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.28515625" style="32" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.7109375" style="33" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.7109375" style="34" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.85546875" style="35" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.28515625" style="36" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.28515625" style="37" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.28515625" style="39" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.28515625" style="40" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.42578125" style="41" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="13.42578125" style="42" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.42578125" style="43" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="14.85546875" style="44" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.140625" style="45" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="9.7109375" style="46" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.85546875" style="47" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.85546875" style="48" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="10.42578125" style="49" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="10.85546875" style="50" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.85546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.42578125" style="52" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="19.85546875" style="53" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="14.85546875" style="54" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="20.28515625" style="55" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="14.140625" style="56" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="5.28515625" style="57" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="6.28515625" style="58" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="11.7109375" style="59" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="15.7109375" style="60" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="17.5703125" style="61" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="16.28515625" style="62" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="9.28515625" style="63" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="12.7109375" style="64" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="15.7109375" style="65" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="15.7109375" style="66" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="15.7109375" style="67" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="15.7109375" style="68" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="12.85546875" style="69" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="13.85546875" style="70" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="10.85546875" style="71" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="15.28515625" style="72" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="14.5703125" style="73" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="10.140625" style="74" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="14.28515625" style="75" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="12.28515625" style="76" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="10.85546875" style="77" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="11.28515625" style="78" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="11.28515625" style="79" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="12.5703125" style="80" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="16.42578125" style="81" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="19.42578125" style="82" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="19.42578125" style="83" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="19.42578125" style="84" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="19.42578125" style="85" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="16.5703125" style="86" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="17.5703125" style="87" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="14.5703125" style="88" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="19" style="89" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="18.28515625" style="90" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="13.85546875" style="91" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="18" style="92" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="16" style="93" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="14.5703125" style="94" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="15" style="95" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="15" style="96" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="7.140625" style="97" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="7.140625" style="98" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="7.140625" style="99" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="7.140625" style="100" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="7.140625" style="101" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="7.140625" style="102" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="7.140625" style="103" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="7.140625" style="104" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="7.140625" style="105" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="7.140625" style="106" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="7.140625" style="107" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="7.140625" style="108" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="7.140625" style="109" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="7.140625" style="110" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="7.140625" style="111" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="7.140625" style="112" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="7.140625" style="113" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="7.140625" style="114" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="7.140625" style="115" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="7.140625" style="116" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="12.7109375" style="117" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="14.7109375" style="118" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="14.7109375" style="119" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="13.7109375" style="120" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="13.7109375" style="121" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="16.85546875" style="122" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="13.85546875" style="123" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="14.7109375" style="124" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="18" style="125" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="13.85546875" style="126" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="14.7109375" style="127" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="18" style="128" bestFit="1" customWidth="1"/>
-    <col min="127" max="127" width="11" style="129" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="14.7109375" style="130" bestFit="1" customWidth="1"/>
-    <col min="129" max="129" width="12.28515625" style="131" bestFit="1" customWidth="1"/>
-    <col min="130" max="130" width="14.28515625" style="132" bestFit="1" customWidth="1"/>
-    <col min="131" max="131" width="19" style="133" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="11.7109375" style="134" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="7.85546875" style="135" bestFit="1" customWidth="1"/>
-    <col min="134" max="134" width="8.28515625" style="136" bestFit="1" customWidth="1"/>
-    <col min="135" max="135" width="14.28515625" style="137" bestFit="1" customWidth="1"/>
-    <col min="136" max="136" width="15.28515625" style="138" bestFit="1" customWidth="1"/>
-    <col min="137" max="137" width="16.7109375" style="139" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="14.42578125" style="140" bestFit="1" customWidth="1"/>
-    <col min="139" max="139" width="18.5703125" style="141" bestFit="1" customWidth="1"/>
-    <col min="140" max="140" width="13.42578125" style="142" bestFit="1" customWidth="1"/>
-    <col min="141" max="141" width="11.28515625" style="143" bestFit="1" customWidth="1"/>
-    <col min="142" max="142" width="16.85546875" style="144" bestFit="1" customWidth="1"/>
-    <col min="143" max="143" width="9.85546875" style="145" bestFit="1" customWidth="1"/>
-    <col min="144" max="144" width="13.5703125" style="146" bestFit="1" customWidth="1"/>
-    <col min="145" max="145" width="14.85546875" style="147" bestFit="1" customWidth="1"/>
-    <col min="146" max="146" width="11.28515625" style="148" bestFit="1" customWidth="1"/>
-    <col min="147" max="147" width="15.85546875" style="149" bestFit="1" customWidth="1"/>
-    <col min="148" max="148" width="8.85546875" style="150" bestFit="1" customWidth="1"/>
-    <col min="149" max="149" width="12.7109375" style="151" bestFit="1" customWidth="1"/>
-    <col min="150" max="150" width="9.140625" style="152" bestFit="1" customWidth="1"/>
-    <col min="151" max="151" width="15" style="153" bestFit="1" customWidth="1"/>
-    <col min="152" max="152" width="18" style="154" bestFit="1" customWidth="1"/>
-    <col min="153" max="153" width="23.28515625" style="155" bestFit="1" customWidth="1"/>
-    <col min="154" max="154" width="10.7109375" style="156" bestFit="1" customWidth="1"/>
-    <col min="155" max="155" width="17.85546875" style="157" bestFit="1" customWidth="1"/>
-    <col min="156" max="156" width="16.140625" style="158" bestFit="1" customWidth="1"/>
-    <col min="157" max="157" width="10.28515625" style="159" bestFit="1" customWidth="1"/>
-    <col min="158" max="158" width="15.42578125" style="160" bestFit="1" customWidth="1"/>
-    <col min="159" max="159" width="11" style="161" bestFit="1" customWidth="1"/>
-    <col min="160" max="160" width="11.28515625" style="162" bestFit="1" customWidth="1"/>
-    <col min="161" max="161" width="19.42578125" style="163" bestFit="1" customWidth="1"/>
-    <col min="162" max="162" width="15.140625" style="164" bestFit="1" customWidth="1"/>
-    <col min="163" max="163" width="23.28515625" style="165" bestFit="1" customWidth="1"/>
-    <col min="164" max="164" width="17.7109375" style="166" bestFit="1" customWidth="1"/>
-    <col min="165" max="165" width="16" style="167" bestFit="1" customWidth="1"/>
-    <col min="166" max="166" width="8" style="168" bestFit="1" customWidth="1"/>
-    <col min="167" max="167" width="10.5703125" style="169" bestFit="1" customWidth="1"/>
-    <col min="168" max="168" width="12.42578125" style="170" bestFit="1" customWidth="1"/>
-    <col min="169" max="169" width="6.42578125" style="171" bestFit="1" customWidth="1"/>
-    <col min="170" max="170" width="9" style="172" bestFit="1" customWidth="1"/>
-    <col min="171" max="171" width="12.5703125" style="173" bestFit="1" customWidth="1"/>
-    <col min="172" max="172" width="14.85546875" style="174" bestFit="1" customWidth="1"/>
-    <col min="173" max="173" width="14.85546875" style="175" bestFit="1" customWidth="1"/>
-    <col min="174" max="174" width="15.42578125" style="176" bestFit="1" customWidth="1"/>
-    <col min="175" max="175" width="10.42578125" style="177" bestFit="1" customWidth="1"/>
-    <col min="176" max="176" width="17.28515625" style="178" bestFit="1" customWidth="1"/>
-    <col min="177" max="177" width="5.42578125" style="179" bestFit="1" customWidth="1"/>
-    <col min="178" max="178" width="18.28515625" style="180" bestFit="1" customWidth="1"/>
-    <col min="179" max="179" width="9.28515625" style="181" bestFit="1" customWidth="1"/>
-    <col min="180" max="180" width="9.7109375" style="182" bestFit="1" customWidth="1"/>
-    <col min="181" max="181" width="6.5703125" style="183" bestFit="1" customWidth="1"/>
-    <col min="182" max="182" width="6.5703125" style="184" bestFit="1" customWidth="1"/>
-    <col min="183" max="183" width="6.5703125" style="185" bestFit="1" customWidth="1"/>
-    <col min="184" max="184" width="6.5703125" style="186" bestFit="1" customWidth="1"/>
-    <col min="185" max="185" width="6.5703125" style="187" bestFit="1" customWidth="1"/>
-    <col min="186" max="186" width="6.5703125" style="188" bestFit="1" customWidth="1"/>
-    <col min="187" max="187" width="18.28515625" style="189" bestFit="1" customWidth="1"/>
-    <col min="188" max="188" width="14.140625" style="190" bestFit="1" customWidth="1"/>
-    <col min="189" max="189" width="16.5703125" style="191" bestFit="1" customWidth="1"/>
-    <col min="190" max="190" width="5.85546875" style="192" bestFit="1" customWidth="1"/>
-    <col min="191" max="191" width="11.7109375" style="193" bestFit="1" customWidth="1"/>
-    <col min="192" max="192" width="9.5703125" style="194" bestFit="1" customWidth="1"/>
-    <col min="193" max="193" width="10" style="195" bestFit="1" customWidth="1"/>
-    <col min="194" max="194" width="10" style="196" bestFit="1" customWidth="1"/>
-    <col min="195" max="195" width="10" style="197" bestFit="1" customWidth="1"/>
-    <col min="196" max="196" width="10" style="198" bestFit="1" customWidth="1"/>
-    <col min="197" max="197" width="10" style="199" bestFit="1" customWidth="1"/>
-    <col min="198" max="198" width="10" style="200" bestFit="1" customWidth="1"/>
-    <col min="199" max="199" width="10" style="201" bestFit="1" customWidth="1"/>
-    <col min="200" max="200" width="10" style="202" bestFit="1" customWidth="1"/>
-    <col min="201" max="201" width="10" style="203" bestFit="1" customWidth="1"/>
-    <col min="202" max="202" width="10" style="204" bestFit="1" customWidth="1"/>
-    <col min="203" max="203" width="10" style="205" bestFit="1" customWidth="1"/>
-    <col min="204" max="204" width="10" style="206" bestFit="1" customWidth="1"/>
-    <col min="205" max="205" width="10.85546875" style="207" bestFit="1" customWidth="1"/>
-    <col min="206" max="206" width="10" style="208" bestFit="1" customWidth="1"/>
-    <col min="207" max="207" width="9" style="209" bestFit="1" customWidth="1"/>
-    <col min="208" max="208" width="13.28515625" style="210" bestFit="1" customWidth="1"/>
-    <col min="209" max="209" width="18" style="211" bestFit="1" customWidth="1"/>
-    <col min="210" max="210" width="14.28515625" style="212" bestFit="1" customWidth="1"/>
-    <col min="211" max="211" width="11.5703125" style="213" bestFit="1" customWidth="1"/>
-    <col min="212" max="212" width="13.140625" style="214" bestFit="1"/>
-    <col min="213" max="213" width="8.5703125" style="215" bestFit="1" customWidth="1"/>
-    <col min="214" max="214" width="11" style="216" bestFit="1" customWidth="1"/>
-    <col min="215" max="215" width="18.5703125" style="217" bestFit="1" customWidth="1"/>
-    <col min="216" max="216" width="23.28515625" style="218" bestFit="1" customWidth="1"/>
-    <col min="217" max="217" width="19.5703125" style="219" bestFit="1" customWidth="1"/>
-    <col min="218" max="218" width="16.85546875" style="220" bestFit="1" customWidth="1"/>
-    <col min="219" max="219" width="18.42578125" style="221" bestFit="1" customWidth="1"/>
-    <col min="220" max="220" width="11.7109375" style="222" bestFit="1" customWidth="1"/>
-    <col min="221" max="221" width="19.5703125" style="223" bestFit="1" customWidth="1"/>
-    <col min="222" max="222" width="15.7109375" style="224" bestFit="1" customWidth="1"/>
-    <col min="223" max="223" width="14" style="225" bestFit="1" customWidth="1"/>
-    <col min="224" max="224" width="12.28515625" style="226" bestFit="1" customWidth="1"/>
-    <col min="225" max="225" width="7.42578125" style="227" bestFit="1" customWidth="1"/>
-    <col min="226" max="226" width="7.28515625" style="228" bestFit="1" customWidth="1"/>
-    <col min="227" max="227" width="8.85546875" style="229" bestFit="1" customWidth="1"/>
-    <col min="228" max="228" width="8.85546875" style="230" bestFit="1" customWidth="1"/>
-    <col min="229" max="229" width="8.85546875" style="231" bestFit="1" customWidth="1"/>
-    <col min="230" max="230" width="8.85546875" style="232" bestFit="1" customWidth="1"/>
-    <col min="231" max="231" width="8.85546875" style="233" bestFit="1" customWidth="1"/>
-    <col min="232" max="232" width="8.85546875" style="234" bestFit="1" customWidth="1"/>
-    <col min="233" max="233" width="8.85546875" style="235" bestFit="1" customWidth="1"/>
-    <col min="234" max="234" width="8.85546875" style="236" bestFit="1" customWidth="1"/>
-    <col min="235" max="235" width="8.85546875" style="237" bestFit="1" customWidth="1"/>
-    <col min="236" max="236" width="8.85546875" style="238" bestFit="1" customWidth="1"/>
-    <col min="237" max="237" width="8.85546875" style="239" bestFit="1" customWidth="1"/>
-    <col min="238" max="238" width="8.85546875" style="240" bestFit="1" customWidth="1"/>
-    <col min="239" max="239" width="8.85546875" style="241" bestFit="1" customWidth="1"/>
-    <col min="240" max="240" width="8.85546875" style="242" bestFit="1" customWidth="1"/>
-    <col min="241" max="241" width="8.85546875" style="243" bestFit="1" customWidth="1"/>
-    <col min="242" max="242" width="8.85546875" style="244" bestFit="1" customWidth="1"/>
-    <col min="243" max="243" width="8.85546875" style="245" bestFit="1" customWidth="1"/>
-    <col min="244" max="244" width="8.85546875" style="246" bestFit="1" customWidth="1"/>
-    <col min="245" max="245" width="8.85546875" style="247" bestFit="1" customWidth="1"/>
-    <col min="246" max="246" width="8.85546875" style="248" bestFit="1" customWidth="1"/>
-    <col min="247" max="247" width="15.85546875" style="249" bestFit="1" customWidth="1"/>
-    <col min="248" max="248" width="17" style="250" bestFit="1" customWidth="1"/>
-    <col min="249" max="249" width="23.5703125" style="251" bestFit="1" customWidth="1"/>
-    <col min="250" max="250" width="8.28515625" style="252" bestFit="1" customWidth="1"/>
-    <col min="251" max="251" width="15.42578125" style="253" bestFit="1" customWidth="1"/>
-    <col min="252" max="252" width="12.5703125" style="254" bestFit="1" customWidth="1"/>
-    <col min="253" max="253" width="11.85546875" style="255" bestFit="1" customWidth="1"/>
-    <col min="254" max="254" width="11.85546875" style="256" bestFit="1" customWidth="1"/>
-    <col min="255" max="255" width="16" style="257" bestFit="1" customWidth="1"/>
-    <col min="256" max="256" width="19.5703125" style="258" bestFit="1" customWidth="1"/>
-    <col min="257" max="257" width="17.28515625" style="259" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="19.85546875" style="260" bestFit="1" customWidth="1"/>
-    <col min="259" max="259" width="17.28515625" style="261" bestFit="1" customWidth="1"/>
-    <col min="260" max="260" width="18.140625" style="262" bestFit="1" customWidth="1"/>
-    <col min="261" max="261" width="15.140625" style="263" bestFit="1" customWidth="1"/>
-    <col min="262" max="262" width="19" style="264" bestFit="1" customWidth="1"/>
-    <col min="263" max="263" width="14" style="265" bestFit="1" customWidth="1"/>
-    <col min="264" max="264" width="13.5703125" style="266" bestFit="1" customWidth="1"/>
-    <col min="265" max="265" width="11" style="267" bestFit="1" customWidth="1"/>
-    <col min="266" max="266" width="20.5703125" style="268" bestFit="1" customWidth="1"/>
-    <col min="267" max="267" width="10.85546875" style="269" bestFit="1" customWidth="1"/>
-    <col min="268" max="268" width="7.85546875" style="270" bestFit="1" customWidth="1"/>
-    <col min="269" max="269" width="7.85546875" style="271" bestFit="1" customWidth="1"/>
-    <col min="270" max="270" width="7.85546875" style="272" bestFit="1" customWidth="1"/>
-    <col min="271" max="271" width="7.85546875" style="273" bestFit="1" customWidth="1"/>
-    <col min="272" max="272" width="7.85546875" style="274" bestFit="1" customWidth="1"/>
-    <col min="273" max="273" width="7.85546875" style="275" bestFit="1" customWidth="1"/>
-    <col min="274" max="274" width="10" style="276" bestFit="1" customWidth="1"/>
-    <col min="275" max="275" width="10" style="277" bestFit="1" customWidth="1"/>
-    <col min="276" max="276" width="10" style="278" bestFit="1" customWidth="1"/>
-    <col min="277" max="277" width="10" style="279" bestFit="1" customWidth="1"/>
-    <col min="278" max="278" width="10" style="280" bestFit="1" customWidth="1"/>
-    <col min="279" max="279" width="10" style="281" bestFit="1" customWidth="1"/>
-    <col min="280" max="280" width="10" style="282" bestFit="1" customWidth="1"/>
-    <col min="281" max="281" width="10" style="283" bestFit="1" customWidth="1"/>
-    <col min="282" max="282" width="10" style="284" bestFit="1" customWidth="1"/>
-    <col min="283" max="283" width="10" style="285" bestFit="1" customWidth="1"/>
-    <col min="284" max="284" width="10" style="286" bestFit="1" customWidth="1"/>
-    <col min="285" max="285" width="10" style="287" bestFit="1" customWidth="1"/>
-    <col min="286" max="286" width="7.42578125" style="288" bestFit="1" customWidth="1"/>
-    <col min="287" max="287" width="16.140625" style="289" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" style="3"/>
+    <col min="2" max="2" width="12" style="4"/>
+    <col min="3" max="3" width="12" style="5"/>
+    <col min="4" max="4" width="12" style="6"/>
+    <col min="5" max="5" width="12" style="7"/>
+    <col min="6" max="6" width="12" style="8"/>
+    <col min="7" max="7" width="12" style="9"/>
+    <col min="8" max="8" width="12" style="10"/>
+    <col min="9" max="9" width="12" style="11"/>
+    <col min="10" max="10" width="12" style="12"/>
+    <col min="11" max="11" width="12" style="13"/>
+    <col min="12" max="12" width="12" style="14"/>
+    <col min="13" max="13" width="12" style="15"/>
+    <col min="14" max="14" width="12" style="16"/>
+    <col min="15" max="15" width="12" style="17"/>
+    <col min="16" max="16" width="12" style="18"/>
+    <col min="17" max="17" width="12" style="19"/>
+    <col min="18" max="18" width="12" style="20"/>
+    <col min="19" max="19" width="12" style="21"/>
+    <col min="20" max="20" width="12" style="22"/>
+    <col min="21" max="21" width="12" style="23"/>
+    <col min="22" max="22" width="12" style="24"/>
+    <col min="23" max="23" width="12" style="25"/>
+    <col min="24" max="24" width="12" style="26"/>
+    <col min="25" max="25" width="12" style="27"/>
+    <col min="26" max="26" width="12" style="28"/>
+    <col min="27" max="27" width="12" style="29"/>
+    <col min="28" max="28" width="12" style="30"/>
+    <col min="29" max="29" width="12" style="31"/>
+    <col min="30" max="30" width="12" style="32"/>
+    <col min="31" max="31" width="12" style="33"/>
+    <col min="32" max="32" width="12" style="34"/>
+    <col min="33" max="33" width="12" style="35"/>
+    <col min="34" max="34" width="12" style="36"/>
+    <col min="35" max="35" width="12" style="37"/>
+    <col min="36" max="36" width="12" style="38"/>
+    <col min="37" max="37" width="12" style="39"/>
+    <col min="38" max="38" width="12" style="40"/>
+    <col min="39" max="39" width="12" style="41"/>
+    <col min="40" max="40" width="12" style="42"/>
+    <col min="41" max="41" width="12" style="43"/>
+    <col min="42" max="42" width="12" style="44"/>
+    <col min="43" max="43" width="12" style="45"/>
+    <col min="44" max="44" width="12" style="46"/>
+    <col min="45" max="45" width="12" style="47"/>
+    <col min="46" max="46" width="12" style="48"/>
+    <col min="47" max="47" width="12" style="49"/>
+    <col min="48" max="48" width="12" style="50"/>
+    <col min="49" max="49" width="12" style="51"/>
+    <col min="50" max="50" width="12" style="52"/>
+    <col min="51" max="51" width="12" style="53"/>
+    <col min="52" max="52" width="12" style="54"/>
+    <col min="53" max="53" width="12" style="55"/>
+    <col min="54" max="54" width="12" style="56"/>
+    <col min="55" max="55" width="12" style="57"/>
+    <col min="56" max="56" width="12" style="58"/>
+    <col min="57" max="57" width="12" style="59"/>
+    <col min="58" max="58" width="12" style="60"/>
+    <col min="59" max="59" width="12" style="61"/>
+    <col min="60" max="60" width="12" style="62"/>
+    <col min="61" max="61" width="12" style="63"/>
+    <col min="62" max="62" width="12" style="64"/>
+    <col min="63" max="63" width="12" style="65"/>
+    <col min="64" max="64" width="12" style="66"/>
+    <col min="65" max="65" width="12" style="67"/>
+    <col min="66" max="66" width="12" style="68"/>
+    <col min="67" max="67" width="12" style="69"/>
+    <col min="68" max="68" width="12" style="70"/>
+    <col min="69" max="69" width="12" style="71"/>
+    <col min="70" max="70" width="12" style="72"/>
+    <col min="71" max="71" width="12" style="73"/>
+    <col min="72" max="72" width="12" style="74"/>
+    <col min="73" max="73" width="12" style="75"/>
+    <col min="74" max="74" width="12" style="76"/>
+    <col min="75" max="75" width="12" style="77"/>
+    <col min="76" max="76" width="12" style="78"/>
+    <col min="77" max="77" width="12" style="79"/>
+    <col min="78" max="78" width="12" style="80"/>
+    <col min="79" max="79" width="12" style="81"/>
+    <col min="80" max="80" width="12" style="82"/>
+    <col min="81" max="81" width="12" style="83"/>
+    <col min="82" max="82" width="12" style="84"/>
+    <col min="83" max="83" width="12" style="85"/>
+    <col min="84" max="84" width="12" style="86"/>
+    <col min="85" max="85" width="12" style="87"/>
+    <col min="86" max="86" width="12" style="88"/>
+    <col min="87" max="87" width="12" style="89"/>
+    <col min="88" max="88" width="12" style="90"/>
+    <col min="89" max="89" width="12" style="91"/>
+    <col min="90" max="90" width="12" style="92"/>
+    <col min="91" max="91" width="12" style="93"/>
+    <col min="92" max="92" width="12" style="94"/>
+    <col min="93" max="93" width="12" style="95"/>
+    <col min="94" max="94" width="12" style="96"/>
+    <col min="95" max="95" width="12" style="97"/>
+    <col min="96" max="96" width="12" style="98"/>
+    <col min="97" max="97" width="12" style="99"/>
+    <col min="98" max="98" width="12" style="100"/>
+    <col min="99" max="99" width="12" style="101"/>
+    <col min="100" max="100" width="12" style="102"/>
+    <col min="101" max="101" width="12" style="103"/>
+    <col min="102" max="102" width="12" style="104"/>
+    <col min="103" max="103" width="12" style="105"/>
+    <col min="104" max="104" width="12" style="106"/>
+    <col min="105" max="105" width="12" style="107"/>
+    <col min="106" max="106" width="12" style="108"/>
+    <col min="107" max="107" width="12" style="109"/>
+    <col min="108" max="108" width="12" style="110"/>
+    <col min="109" max="109" width="12" style="111"/>
+    <col min="110" max="110" width="12" style="112"/>
+    <col min="111" max="111" width="12" style="113"/>
+    <col min="112" max="112" width="12" style="114"/>
+    <col min="113" max="113" width="12" style="115"/>
+    <col min="114" max="114" width="12" style="116"/>
+    <col min="115" max="115" width="12" style="117"/>
+    <col min="116" max="116" width="12" style="118"/>
+    <col min="117" max="117" width="12" style="119"/>
+    <col min="118" max="118" width="12" style="120"/>
+    <col min="119" max="119" width="12" style="121"/>
+    <col min="120" max="120" width="12" style="122"/>
+    <col min="121" max="121" width="12" style="123"/>
+    <col min="122" max="122" width="12" style="124"/>
+    <col min="123" max="123" width="12" style="125"/>
+    <col min="124" max="124" width="12" style="126"/>
+    <col min="125" max="125" width="12" style="127"/>
+    <col min="126" max="126" width="12" style="128"/>
+    <col min="127" max="127" width="12" style="129"/>
+    <col min="128" max="128" width="12" style="130"/>
+    <col min="129" max="129" width="12" style="131"/>
+    <col min="130" max="130" width="12" style="132"/>
+    <col min="131" max="131" width="12" style="133"/>
+    <col min="132" max="132" width="12" style="134"/>
+    <col min="133" max="133" width="12" style="135"/>
+    <col min="134" max="134" width="12" style="136"/>
+    <col min="135" max="135" width="12" style="137"/>
+    <col min="136" max="136" width="12" style="138"/>
+    <col min="137" max="137" width="12" style="139"/>
+    <col min="138" max="138" width="12" style="140"/>
+    <col min="139" max="139" width="12" style="141"/>
+    <col min="140" max="140" width="12" style="142"/>
+    <col min="141" max="141" width="12" style="143"/>
+    <col min="142" max="142" width="12" style="144"/>
+    <col min="143" max="143" width="12" style="145"/>
+    <col min="144" max="144" width="12" style="146"/>
+    <col min="145" max="145" width="12" style="147"/>
+    <col min="146" max="146" width="12" style="148"/>
+    <col min="147" max="147" width="12" style="149"/>
+    <col min="148" max="148" width="12" style="150"/>
+    <col min="149" max="149" width="12" style="151"/>
+    <col min="150" max="150" width="12" style="152"/>
+    <col min="151" max="151" width="12" style="153"/>
+    <col min="152" max="152" width="12" style="154"/>
+    <col min="153" max="153" width="12" style="155"/>
+    <col min="154" max="154" width="12" style="156"/>
+    <col min="155" max="155" width="12" style="157"/>
+    <col min="156" max="156" width="12" style="158"/>
+    <col min="157" max="157" width="12" style="159"/>
+    <col min="158" max="158" width="12" style="160"/>
+    <col min="159" max="159" width="12" style="161"/>
+    <col min="160" max="160" width="12" style="162"/>
+    <col min="161" max="161" width="12" style="163"/>
+    <col min="162" max="162" width="12" style="164"/>
+    <col min="163" max="163" width="12" style="165"/>
+    <col min="164" max="164" width="12" style="166"/>
+    <col min="165" max="165" width="12" style="167"/>
+    <col min="166" max="166" width="12" style="168"/>
+    <col min="167" max="167" width="12" style="169"/>
+    <col min="168" max="168" width="12" style="170"/>
+    <col min="169" max="169" width="12" style="171"/>
+    <col min="170" max="170" width="12" style="172"/>
+    <col min="171" max="171" width="12" style="173"/>
+    <col min="172" max="172" width="12" style="174"/>
+    <col min="173" max="173" width="12" style="175"/>
+    <col min="174" max="174" width="12" style="176"/>
+    <col min="175" max="175" width="12" style="177"/>
+    <col min="176" max="176" width="12" style="178"/>
+    <col min="177" max="177" width="12" style="179"/>
+    <col min="178" max="178" width="12" style="180"/>
+    <col min="179" max="179" width="12" style="181"/>
+    <col min="180" max="180" width="12" style="182"/>
+    <col min="181" max="181" width="12" style="183"/>
+    <col min="182" max="182" width="12" style="184"/>
+    <col min="183" max="183" width="12" style="185"/>
+    <col min="184" max="184" width="12" style="186"/>
+    <col min="185" max="185" width="12" style="187"/>
+    <col min="186" max="186" width="12" style="188"/>
+    <col min="187" max="187" width="12" style="189"/>
+    <col min="188" max="188" width="12" style="190"/>
+    <col min="189" max="189" width="12" style="191"/>
+    <col min="190" max="190" width="12" style="192"/>
+    <col min="191" max="191" width="12" style="193"/>
+    <col min="192" max="192" width="12" style="194"/>
+    <col min="193" max="193" width="12" style="195"/>
+    <col min="194" max="194" width="12" style="196"/>
+    <col min="195" max="195" width="12" style="197"/>
+    <col min="196" max="196" width="12" style="198"/>
+    <col min="197" max="197" width="12" style="199"/>
+    <col min="198" max="198" width="12" style="200"/>
+    <col min="199" max="199" width="12" style="201"/>
+    <col min="200" max="200" width="12" style="202"/>
+    <col min="201" max="201" width="12" style="203"/>
+    <col min="202" max="202" width="12" style="204"/>
+    <col min="203" max="203" width="12" style="205"/>
+    <col min="204" max="204" width="12" style="206"/>
+    <col min="205" max="205" width="12" style="207"/>
+    <col min="206" max="206" width="12" style="208"/>
+    <col min="207" max="207" width="12" style="209"/>
+    <col min="208" max="208" width="12" style="210"/>
+    <col min="209" max="209" width="12" style="211"/>
+    <col min="210" max="210" width="12" style="212"/>
+    <col min="211" max="211" width="12" style="213"/>
+    <col min="212" max="212" width="12" style="214"/>
+    <col min="213" max="213" width="12" style="215"/>
+    <col min="214" max="214" width="12" style="216"/>
+    <col min="215" max="215" width="12" style="217"/>
+    <col min="216" max="216" width="12" style="218"/>
+    <col min="217" max="217" width="12" style="219"/>
+    <col min="218" max="218" width="12" style="220"/>
+    <col min="219" max="219" width="12" style="221"/>
+    <col min="220" max="220" width="12" style="222"/>
+    <col min="221" max="221" width="12" style="223"/>
+    <col min="222" max="222" width="12" style="224"/>
+    <col min="223" max="223" width="12" style="225"/>
+    <col min="224" max="224" width="12" style="226"/>
+    <col min="225" max="225" width="12" style="227"/>
+    <col min="226" max="226" width="12" style="228"/>
+    <col min="227" max="227" width="12" style="229"/>
+    <col min="228" max="228" width="12" style="230"/>
+    <col min="229" max="229" width="12" style="231"/>
+    <col min="230" max="230" width="12" style="232"/>
+    <col min="231" max="231" width="12" style="233"/>
+    <col min="232" max="232" width="12" style="234"/>
+    <col min="233" max="233" width="12" style="235"/>
+    <col min="234" max="234" width="12" style="236"/>
+    <col min="235" max="235" width="12" style="237"/>
+    <col min="236" max="236" width="12" style="238"/>
+    <col min="237" max="237" width="12" style="239"/>
+    <col min="238" max="238" width="12" style="240"/>
+    <col min="239" max="239" width="12" style="241"/>
+    <col min="240" max="240" width="12" style="242"/>
+    <col min="241" max="241" width="12" style="243"/>
+    <col min="242" max="242" width="12" style="244"/>
+    <col min="243" max="243" width="12" style="245"/>
+    <col min="244" max="244" width="12" style="246"/>
+    <col min="245" max="245" width="12" style="247"/>
+    <col min="246" max="246" width="12" style="248"/>
+    <col min="247" max="247" width="12" style="249"/>
+    <col min="248" max="248" width="12" style="250"/>
+    <col min="249" max="249" width="12" style="251"/>
+    <col min="250" max="250" width="12" style="252"/>
+    <col min="251" max="251" width="12" style="253"/>
+    <col min="252" max="252" width="12" style="254"/>
+    <col min="253" max="253" width="12" style="255"/>
+    <col min="254" max="254" width="12" style="256"/>
+    <col min="255" max="255" width="12" style="257"/>
+    <col min="256" max="256" width="12" style="258"/>
+    <col min="257" max="257" width="12" style="259"/>
+    <col min="258" max="258" width="12" style="260"/>
+    <col min="259" max="259" width="12" style="261"/>
+    <col min="260" max="260" width="12" style="262"/>
+    <col min="261" max="261" width="12" style="263"/>
+    <col min="262" max="262" width="12" style="264"/>
+    <col min="263" max="263" width="12" style="265"/>
+    <col min="264" max="264" width="12" style="266"/>
+    <col min="265" max="265" width="12" style="267"/>
+    <col min="266" max="266" width="12" style="268"/>
+    <col min="267" max="267" width="12" style="269"/>
+    <col min="268" max="268" width="12" style="270"/>
+    <col min="269" max="269" width="12" style="271"/>
+    <col min="270" max="270" width="12" style="272"/>
+    <col min="271" max="271" width="12" style="273"/>
+    <col min="272" max="272" width="12" style="274"/>
+    <col min="273" max="273" width="12" style="275"/>
+    <col min="274" max="274" width="12" style="276"/>
+    <col min="275" max="275" width="12" style="277"/>
+    <col min="276" max="276" width="12" style="278"/>
+    <col min="277" max="277" width="12" style="279"/>
+    <col min="278" max="278" width="12" style="280"/>
+    <col min="279" max="279" width="12" style="281"/>
+    <col min="280" max="280" width="12" style="282"/>
+    <col min="281" max="281" width="12" style="283"/>
+    <col min="282" max="282" width="12" style="284"/>
+    <col min="283" max="283" width="12" style="285"/>
+    <col min="284" max="284" width="12" style="286"/>
+    <col min="285" max="285" width="12" style="287"/>
+    <col min="286" max="286" width="12" style="288"/>
+    <col min="287" max="287" width="12" style="289"/>
+    <col min="288" max="288" width="12" style="290"/>
+    <col min="289" max="289" width="12" style="291"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:287" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:289" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2750,7 +2866,7 @@
         <v>28</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>561</v>
+        <v>30</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>32</v>
@@ -2936,637 +3052,643 @@
         <v>152</v>
       </c>
       <c r="BZ1" s="1" t="s">
-        <v>30</v>
+        <v>154</v>
       </c>
       <c r="CA1" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="CB1" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="CC1" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="CD1" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="CE1" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CF1" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="CG1" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="CH1" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="CI1" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="CJ1" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="CK1" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="CL1" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="CM1" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="CN1" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="CO1" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="CP1" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="CQ1" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="CR1" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="CS1" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="CT1" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="CU1" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="CV1" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="CW1" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="CX1" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="CY1" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="CZ1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="DA1" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="DB1" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="DC1" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="DD1" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="DE1" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="DF1" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="DG1" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="DH1" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="DI1" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="DJ1" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="DK1" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="DL1" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="DM1" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="DN1" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="DO1" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="DP1" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="DQ1" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="DR1" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="DS1" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="DT1" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="DU1" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="DV1" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="DW1" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="DX1" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="DY1" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="DZ1" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="EA1" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="EB1" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="EC1" s="1" t="s">
-        <v>263</v>
+        <v>256</v>
+      </c>
+      <c r="DZ1" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="EA1" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="EB1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="EC1" s="2" t="s">
+        <v>264</v>
       </c>
       <c r="ED1" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="EE1" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="EF1" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="EG1" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="EH1" s="2" t="s">
-        <v>273</v>
+        <v>268</v>
+      </c>
+      <c r="EF1" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="EG1" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="EH1" s="1" t="s">
+        <v>274</v>
       </c>
       <c r="EI1" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="EJ1" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="EK1" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="EL1" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="EM1" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="EN1" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="EO1" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
+      </c>
+      <c r="EO1" s="2" t="s">
+        <v>288</v>
       </c>
       <c r="EP1" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="EQ1" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="ER1" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
+      </c>
+      <c r="ER1" s="1" t="s">
+        <v>294</v>
       </c>
       <c r="ES1" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="ET1" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="EU1" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="EV1" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="EW1" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
+      </c>
+      <c r="EW1" s="2" t="s">
+        <v>304</v>
       </c>
       <c r="EX1" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="EY1" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="EZ1" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="FA1" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="FB1" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="FC1" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
+      </c>
+      <c r="FC1" s="1" t="s">
+        <v>316</v>
       </c>
       <c r="FD1" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="FE1" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="FF1" s="2" t="s">
-        <v>321</v>
+        <v>318</v>
+      </c>
+      <c r="FE1" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="FF1" s="1" t="s">
+        <v>322</v>
       </c>
       <c r="FG1" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="FH1" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="FI1" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="FJ1" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="FK1" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="FL1" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="FM1" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="FN1" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="FO1" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="FP1" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="FQ1" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="FR1" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="FS1" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
+      </c>
+      <c r="FS1" s="2" t="s">
+        <v>348</v>
       </c>
       <c r="FT1" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="FU1" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="FV1" s="2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="FW1" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="FX1" s="1" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="FY1" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="FZ1" s="1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="GA1" s="1" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="GB1" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="GC1" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="GD1" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
+      </c>
+      <c r="GD1" s="2" t="s">
+        <v>370</v>
       </c>
       <c r="GE1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="GF1" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="GG1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="GH1" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="GI1" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="GJ1" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="GK1" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="GL1" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="GM1" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="GN1" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="GO1" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="GP1" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="GQ1" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="GR1" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="GS1" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="GT1" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="GU1" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="GV1" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="GW1" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="GX1" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="GY1" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="GZ1" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="HA1" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="HB1" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="HC1" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="HD1" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="HE1" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="HF1" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="HG1" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="HH1" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="HI1" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="HJ1" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="HK1" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="HL1" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="HM1" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="HN1" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="HO1" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="HP1" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="HQ1" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="HR1" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="HS1" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="HT1" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="HU1" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="HV1" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="HW1" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="HX1" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="HY1" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="HZ1" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="IA1" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="IB1" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="IC1" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="ID1" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="IE1" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="IF1" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="IG1" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="IH1" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="II1" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="IJ1" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="IK1" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="IL1" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="IM1" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="IN1" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="IO1" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="IP1" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="IQ1" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="IR1" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="IS1" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="IT1" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="IU1" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="IV1" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="IW1" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="IX1" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="IY1" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="IZ1" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="JA1" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="JB1" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="JC1" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="JD1" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="JE1" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="JF1" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="JG1" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="JH1" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="JI1" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="JJ1" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="JK1" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="JL1" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="JM1" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="JN1" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="JO1" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="JP1" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="JQ1" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="JR1" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="JS1" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="JT1" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="JU1" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="JV1" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="JW1" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="JX1" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="JY1" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="JZ1" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="KA1" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="KB1" s="1" t="s">
         <v>562</v>
       </c>
-      <c r="GF1" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="GG1" s="2" t="s">
-        <v>563</v>
-      </c>
-      <c r="GH1" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="GI1" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="GJ1" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="GK1" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="GL1" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="GM1" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="GN1" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="GO1" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="GP1" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="GQ1" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="GR1" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="GS1" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="GT1" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="GU1" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="GV1" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="GW1" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="GX1" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="GY1" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="GZ1" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="HA1" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="HB1" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="HC1" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="HD1" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="HE1" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="HF1" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="HG1" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="HH1" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="HI1" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="HJ1" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="HK1" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="HL1" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="HM1" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="HN1" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="HO1" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="HP1" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="HQ1" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="HR1" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="HS1" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="HT1" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="HU1" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="HV1" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="HW1" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="HX1" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="HY1" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="HZ1" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="IA1" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="IB1" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="IC1" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="ID1" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="IE1" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="IF1" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="IG1" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="IH1" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="II1" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="IJ1" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="IK1" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="IL1" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="IM1" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="IN1" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="IO1" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="IP1" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="IQ1" s="2" t="s">
+      <c r="KC1" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="IR1" s="1" t="s">
-        <v>565</v>
-      </c>
-      <c r="IS1" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="IT1" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="IU1" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="IV1" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="IW1" s="2" t="s">
-        <v>507</v>
-      </c>
-      <c r="IX1" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="IY1" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="IZ1" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="JA1" s="1" t="s">
-        <v>566</v>
-      </c>
-      <c r="JB1" s="1" t="s">
-        <v>516</v>
-      </c>
-      <c r="JC1" s="2" t="s">
-        <v>518</v>
-      </c>
-      <c r="JD1" s="2" t="s">
-        <v>520</v>
-      </c>
-      <c r="JE1" s="2" t="s">
-        <v>522</v>
-      </c>
-      <c r="JF1" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="JG1" s="1" t="s">
-        <v>567</v>
-      </c>
-      <c r="JH1" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="JI1" s="1" t="s">
-        <v>569</v>
-      </c>
-      <c r="JJ1" s="1" t="s">
-        <v>570</v>
-      </c>
-      <c r="JK1" s="1" t="s">
-        <v>571</v>
-      </c>
-      <c r="JL1" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="JM1" s="1" t="s">
-        <v>573</v>
-      </c>
-      <c r="JN1" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="JO1" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="JP1" s="1" t="s">
-        <v>537</v>
-      </c>
-      <c r="JQ1" s="1" t="s">
-        <v>539</v>
-      </c>
-      <c r="JR1" s="1" t="s">
-        <v>541</v>
-      </c>
-      <c r="JS1" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="JT1" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="JU1" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="JV1" s="1" t="s">
-        <v>549</v>
-      </c>
-      <c r="JW1" s="1" t="s">
-        <v>551</v>
-      </c>
-      <c r="JX1" s="1" t="s">
-        <v>553</v>
-      </c>
-      <c r="JY1" s="1" t="s">
-        <v>555</v>
-      </c>
-      <c r="JZ1" s="1" t="s">
-        <v>557</v>
-      </c>
-      <c r="KA1" s="1" t="s">
-        <v>559</v>
-      </c>
     </row>
-    <row r="2" spans="1:287" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:289" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -3799,638 +3921,644 @@
         <v>153</v>
       </c>
       <c r="BZ2" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="CA2" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="CB2" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="CC2" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="CD2" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="CE2" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="CF2" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="CG2" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="CH2" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="CI2" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="CJ2" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="CK2" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="CL2" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="CM2" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="CN2" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CO2" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="CP2" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CQ2" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="CR2" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="CS2" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="CT2" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="CU2" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="CV2" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="CW2" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="CX2" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="CY2" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="CZ2" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="DA2" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="DB2" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="DC2" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="DD2" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="DE2" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="DF2" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="DG2" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="DH2" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="DI2" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="DJ2" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="DK2" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="DL2" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="DM2" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="DN2" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="DO2" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="DP2" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="DQ2" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="DR2" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="DS2" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="DT2" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="DU2" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="DV2" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="DW2" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="DX2" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="DY2" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="DZ2" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="EA2" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="EB2" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="EC2" s="1" t="s">
-        <v>264</v>
+        <v>257</v>
+      </c>
+      <c r="DZ2" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="EA2" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="EB2" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="EC2" s="2" t="s">
+        <v>265</v>
       </c>
       <c r="ED2" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="EE2" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="EF2" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="EG2" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="EH2" s="2" t="s">
-        <v>274</v>
+        <v>269</v>
+      </c>
+      <c r="EF2" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="EG2" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="EH2" s="1" t="s">
+        <v>275</v>
       </c>
       <c r="EI2" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="EJ2" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="EK2" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="EL2" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="EM2" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="EN2" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="EO2" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
+      </c>
+      <c r="EO2" s="2" t="s">
+        <v>289</v>
       </c>
       <c r="EP2" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="EQ2" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="ER2" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
+      </c>
+      <c r="ER2" s="1" t="s">
+        <v>295</v>
       </c>
       <c r="ES2" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="ET2" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="EU2" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="EV2" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="EW2" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
+      </c>
+      <c r="EW2" s="2" t="s">
+        <v>305</v>
       </c>
       <c r="EX2" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="EY2" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="EZ2" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="FA2" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="FB2" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="FC2" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
+      </c>
+      <c r="FC2" s="1" t="s">
+        <v>317</v>
       </c>
       <c r="FD2" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="FE2" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="FF2" s="2" t="s">
-        <v>322</v>
+        <v>319</v>
+      </c>
+      <c r="FE2" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="FF2" s="1" t="s">
+        <v>323</v>
       </c>
       <c r="FG2" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="FH2" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="FI2" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="FJ2" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="FK2" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="FL2" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="FM2" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="FN2" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="FO2" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="FP2" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="FQ2" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="FR2" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="FS2" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
+      </c>
+      <c r="FS2" s="2" t="s">
+        <v>349</v>
       </c>
       <c r="FT2" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="FU2" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="FV2" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="FW2" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="FX2" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="FY2" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="FZ2" s="1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="GA2" s="1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="GB2" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="GC2" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="GD2" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
+      </c>
+      <c r="GD2" s="2" t="s">
+        <v>371</v>
       </c>
       <c r="GE2" s="2" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="GF2" s="2" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="GG2" s="2" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="GH2" s="2" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="GI2" s="2" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="GJ2" s="1" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="GK2" s="1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="GL2" s="1" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="GM2" s="1" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="GN2" s="1" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="GO2" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="GP2" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="GQ2" s="1" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="GR2" s="1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="GS2" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="GT2" s="1" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="GU2" s="1" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="GV2" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="GW2" s="1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="GX2" s="1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="GY2" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="GZ2" s="2" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="HA2" s="2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="HB2" s="2" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="HC2" s="2" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="HD2" s="2" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="HE2" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="HF2" s="2" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="HG2" s="1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="HH2" s="2" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="HI2" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="HJ2" s="2" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="HK2" s="2" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="HL2" s="1" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="HM2" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="HN2" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="HO2" s="2" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="HP2" s="2" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="HQ2" s="2" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="HR2" s="2" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="HS2" s="1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="HT2" s="1" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="HU2" s="1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="HV2" s="1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="HW2" s="1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="HX2" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="HY2" s="1" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="HZ2" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="IA2" s="1" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="IB2" s="1" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="IC2" s="1" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="ID2" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="IE2" s="1" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="IF2" s="1" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="IG2" s="1" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="IH2" s="1" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="II2" s="1" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="IJ2" s="1" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="IK2" s="1" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="IL2" s="1" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="IM2" s="1" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="IN2" s="1" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="IO2" s="1" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="IP2" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="IQ2" s="2" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="IR2" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="IS2" s="1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="IT2" s="1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="IU2" s="2" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="IV2" s="1" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="IW2" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="IX2" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="IY2" s="2" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="IZ2" s="1" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="JA2" s="1" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="JB2" s="1" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="JC2" s="2" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="JD2" s="2" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="JE2" s="2" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="JF2" s="1" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="JG2" s="1" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="JH2" s="1" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="JI2" s="1" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="JJ2" s="1" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="JK2" s="1" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="JL2" s="1" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="JM2" s="1" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="JN2" s="1" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="JO2" s="1" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="JP2" s="1" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="JQ2" s="1" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="JR2" s="1" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="JS2" s="1" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="JT2" s="1" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="JU2" s="1" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="JV2" s="1" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="JW2" s="1" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="JX2" s="1" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="JY2" s="1" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="JZ2" s="1" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="KA2" s="1" t="s">
-        <v>560</v>
+        <v>561</v>
+      </c>
+      <c r="KB2" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="KC2" s="1" t="s">
+        <v>565</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
To deploy enhancement, except SKU validation
</commit_message>
<xml_diff>
--- a/files/temporaryTemplates/TempOrderHoneywell.xlsx
+++ b/files/temporaryTemplates/TempOrderHoneywell.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Reports\ConversionToolExcelToExcel\temporaryTemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Reports\conversionToolBack\files\temporaryTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A12307-9B37-4B4A-B75A-6C3E8E340470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB4B36F1-C7D8-4395-A7A4-2693B99546E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,8 +19,144 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>FLUX</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Date FormatYYYY-MM-DD</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Date FormatYYYY-MM-DD</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Date FormatYYYY-MM-DD</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Date FormatYYYY-MM-DD</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DL1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Date FormatYYYY-MM-DD</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DM1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Date FormatYYYY-MM-DD</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DN1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Date FormatYYYY-MM-DD</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EH1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Date FormatYYYY-MM-DD</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EK1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Date FormatYYYY-MM-DD</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="566">
   <si>
     <t>Warehouse ID</t>
   </si>
@@ -304,13 +440,13 @@
     <t>billingFax</t>
   </si>
   <si>
-    <t>Billing TEL1</t>
+    <t>Billing Telphone1</t>
   </si>
   <si>
     <t>billingTel1</t>
   </si>
   <si>
-    <t>Billing TEL2</t>
+    <t>Billing Telphone2</t>
   </si>
   <si>
     <t>billingTel2</t>
@@ -472,18 +608,21 @@
     <t>carrierFax</t>
   </si>
   <si>
-    <t>Carrier TEL1</t>
+    <t>Carrier Telphone1</t>
   </si>
   <si>
     <t>carrierTel1</t>
   </si>
   <si>
-    <t>Carrier TEL2</t>
+    <t>Carrier Telphone2</t>
   </si>
   <si>
     <t>carrierTel2</t>
   </si>
   <si>
+    <t>Issue Party ID</t>
+  </si>
+  <si>
     <t>issuePartyId</t>
   </si>
   <si>
@@ -571,13 +710,13 @@
     <t>issuePartyFax</t>
   </si>
   <si>
-    <t>Issue Party TEL1</t>
+    <t>Issue Party Telphone1</t>
   </si>
   <si>
     <t>issuePartyTel1</t>
   </si>
   <si>
-    <t>Issue Party TEL2</t>
+    <t>Issue Party Telphone2</t>
   </si>
   <si>
     <t>issuePartyTel2</t>
@@ -781,318 +920,312 @@
     <t>rfGetTask</t>
   </si>
   <si>
-    <t>ERP Cancel Flag</t>
+    <t>Single Match</t>
+  </si>
+  <si>
+    <t>singleMatch</t>
+  </si>
+  <si>
+    <t>SerialNO Catch</t>
+  </si>
+  <si>
+    <t>serialNoCatch</t>
+  </si>
+  <si>
+    <t>Require DeliveryNO</t>
+  </si>
+  <si>
+    <t>requireDeliveryNo</t>
+  </si>
+  <si>
+    <t>Archive Flag</t>
+  </si>
+  <si>
+    <t>archiveFlag</t>
+  </si>
+  <si>
+    <t>Allow Partial Allocation</t>
+  </si>
+  <si>
+    <t>ful_alc</t>
+  </si>
+  <si>
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>channel</t>
+  </si>
+  <si>
+    <t>Weighting Flag</t>
+  </si>
+  <si>
+    <t>weightingFlag</t>
+  </si>
+  <si>
+    <t>Allow Shipment</t>
+  </si>
+  <si>
+    <t>allowShipment</t>
+  </si>
+  <si>
+    <t>Allow Partial Ship</t>
+  </si>
+  <si>
+    <t>allowPartialShip</t>
+  </si>
+  <si>
+    <t>EDI Carrier Flag</t>
+  </si>
+  <si>
+    <t>ediCarrierFlag</t>
+  </si>
+  <si>
+    <t>Last Shipment Time</t>
+  </si>
+  <si>
+    <t>lastShipmentTime</t>
+  </si>
+  <si>
+    <t>Create Source</t>
+  </si>
+  <si>
+    <t>createSource</t>
+  </si>
+  <si>
+    <t>Zone Group</t>
+  </si>
+  <si>
+    <t>zoneGroup</t>
+  </si>
+  <si>
+    <t>Medical Xml Time</t>
+  </si>
+  <si>
+    <t>medicalXmlTime</t>
+  </si>
+  <si>
+    <t>Follow Up</t>
+  </si>
+  <si>
+    <t>followUp</t>
+  </si>
+  <si>
+    <t>Sales Orderno</t>
+  </si>
+  <si>
+    <t>salesOrderNo</t>
+  </si>
+  <si>
+    <t>Put Location TO</t>
+  </si>
+  <si>
+    <t>putToLocation</t>
+  </si>
+  <si>
+    <t>DeliveryNO</t>
+  </si>
+  <si>
+    <t>deliveryNo</t>
+  </si>
+  <si>
+    <t>Allocation Count</t>
+  </si>
+  <si>
+    <t>allocationCount</t>
+  </si>
+  <si>
+    <t>WaveNO</t>
+  </si>
+  <si>
+    <t>waveNo</t>
+  </si>
+  <si>
+    <t>Carton Group</t>
+  </si>
+  <si>
+    <t>cartonGroup</t>
+  </si>
+  <si>
+    <t>Carton ID</t>
+  </si>
+  <si>
+    <t>cartonId</t>
+  </si>
+  <si>
+    <t>Order GroupNO</t>
+  </si>
+  <si>
+    <t>orderGroupNo</t>
+  </si>
+  <si>
+    <t>Trans Service Level</t>
+  </si>
+  <si>
+    <t>transServiceLevel</t>
+  </si>
+  <si>
+    <t>Order Handle Instruction</t>
+  </si>
+  <si>
+    <t>orderHandleInstruction</t>
+  </si>
+  <si>
+    <t>Total Cubic</t>
+  </si>
+  <si>
+    <t>totalCubic</t>
+  </si>
+  <si>
+    <t>Total Gross Weight</t>
+  </si>
+  <si>
+    <t>totalGrossWeight</t>
+  </si>
+  <si>
+    <t>Total Net Weight</t>
+  </si>
+  <si>
+    <t>totalNetWeight</t>
+  </si>
+  <si>
+    <t>Total Price</t>
+  </si>
+  <si>
+    <t>totalPrice</t>
+  </si>
+  <si>
+    <t>Total Line Count</t>
+  </si>
+  <si>
+    <t>totalLineCount</t>
+  </si>
+  <si>
+    <t>Cur LineNO</t>
+  </si>
+  <si>
+    <t>curLineNo</t>
+  </si>
+  <si>
+    <t>Parcel Mark</t>
+  </si>
+  <si>
+    <t>parcelMark</t>
+  </si>
+  <si>
+    <t>Parcel Consolidation</t>
+  </si>
+  <si>
+    <t>parcelConsolidation</t>
+  </si>
+  <si>
+    <t>Total SKU Count</t>
+  </si>
+  <si>
+    <t>totalSkuCount</t>
+  </si>
+  <si>
+    <t>Warehouse Transfer Flag</t>
+  </si>
+  <si>
+    <t>warehouseTransferFlag</t>
+  </si>
+  <si>
+    <t>Express Platform</t>
+  </si>
+  <si>
+    <t>expressPlatform</t>
+  </si>
+  <si>
+    <t>OCP NO</t>
+  </si>
+  <si>
+    <t>ocpNo</t>
+  </si>
+  <si>
+    <t>VehicleNO</t>
+  </si>
+  <si>
+    <t>vehicleNo</t>
+  </si>
+  <si>
+    <t>Vehicle Type</t>
+  </si>
+  <si>
+    <t>vehicleType</t>
+  </si>
+  <si>
+    <t>Driver</t>
+  </si>
+  <si>
+    <t>driver</t>
+  </si>
+  <si>
+    <t>Split Flag</t>
+  </si>
+  <si>
+    <t>splitFlag</t>
+  </si>
+  <si>
+    <t>Loc Group1 List</t>
+  </si>
+  <si>
+    <t>locGroup1List</t>
+  </si>
+  <si>
+    <t>Loc Group2 List</t>
+  </si>
+  <si>
+    <t>locGroup2List</t>
+  </si>
+  <si>
+    <t>Shipment Count</t>
+  </si>
+  <si>
+    <t>shipmentCount</t>
+  </si>
+  <si>
+    <t>Wave Rule</t>
+  </si>
+  <si>
+    <t>waveRule</t>
+  </si>
+  <si>
+    <t>Reverse Order NO</t>
+  </si>
+  <si>
+    <t>reverseOrderNo</t>
+  </si>
+  <si>
+    <t>Shop</t>
+  </si>
+  <si>
+    <t>shop</t>
+  </si>
+  <si>
+    <t>Replenish Group ID</t>
+  </si>
+  <si>
+    <t>rpGroupId</t>
+  </si>
+  <si>
+    <t>Total QTY</t>
+  </si>
+  <si>
+    <t>totalQty</t>
+  </si>
+  <si>
+    <t>Crossdock Flag</t>
+  </si>
+  <si>
+    <t>crossdockFlag</t>
+  </si>
+  <si>
+    <t>Erp Cancel Flag</t>
   </si>
   <si>
     <t>erpCancelFlag</t>
   </si>
   <si>
-    <t>Single Match</t>
-  </si>
-  <si>
-    <t>singleMatch</t>
-  </si>
-  <si>
-    <t>SerialNO Catch</t>
-  </si>
-  <si>
-    <t>serialNoCatch</t>
-  </si>
-  <si>
-    <t>Require DeliveryNO</t>
-  </si>
-  <si>
-    <t>requireDeliveryNo</t>
-  </si>
-  <si>
-    <t>Archive Flag</t>
-  </si>
-  <si>
-    <t>archiveFlag</t>
-  </si>
-  <si>
-    <t>FUL ALC</t>
-  </si>
-  <si>
-    <t>ful_alc</t>
-  </si>
-  <si>
-    <t>Channel</t>
-  </si>
-  <si>
-    <t>channel</t>
-  </si>
-  <si>
-    <t>Weighting Flag</t>
-  </si>
-  <si>
-    <t>weightingFlag</t>
-  </si>
-  <si>
-    <t>Allow Shipment</t>
-  </si>
-  <si>
-    <t>allowShipment</t>
-  </si>
-  <si>
-    <t>Allow Partial Ship</t>
-  </si>
-  <si>
-    <t>allowPartialShip</t>
-  </si>
-  <si>
-    <t>EDI Carrier Flag</t>
-  </si>
-  <si>
-    <t>ediCarrierFlag</t>
-  </si>
-  <si>
-    <t>Last Shipment Time</t>
-  </si>
-  <si>
-    <t>lastShipmentTime</t>
-  </si>
-  <si>
-    <t>Create Source</t>
-  </si>
-  <si>
-    <t>createSource</t>
-  </si>
-  <si>
-    <t>Zone Group</t>
-  </si>
-  <si>
-    <t>zoneGroup</t>
-  </si>
-  <si>
-    <t>Medical Xml Time</t>
-  </si>
-  <si>
-    <t>medicalXmlTime</t>
-  </si>
-  <si>
-    <t>Follow Up</t>
-  </si>
-  <si>
-    <t>followUp</t>
-  </si>
-  <si>
-    <t>Sales Orderno</t>
-  </si>
-  <si>
-    <t>salesOrderno</t>
-  </si>
-  <si>
-    <t>Put Location TO</t>
-  </si>
-  <si>
-    <t>putToLocation</t>
-  </si>
-  <si>
-    <t>DeliveryNO</t>
-  </si>
-  <si>
-    <t>deliveryNo</t>
-  </si>
-  <si>
-    <t>Allocation Count</t>
-  </si>
-  <si>
-    <t>allocationCount</t>
-  </si>
-  <si>
-    <t>WaveNO</t>
-  </si>
-  <si>
-    <t>waveNo</t>
-  </si>
-  <si>
-    <t>Carton Group</t>
-  </si>
-  <si>
-    <t>cartonGroup</t>
-  </si>
-  <si>
-    <t>Carton ID</t>
-  </si>
-  <si>
-    <t>cartonId</t>
-  </si>
-  <si>
-    <t>Order GroupNO</t>
-  </si>
-  <si>
-    <t>orderGroupNo</t>
-  </si>
-  <si>
-    <t>Trans Service Level</t>
-  </si>
-  <si>
-    <t>transServiceLevel</t>
-  </si>
-  <si>
-    <t>Order Handle Instruction</t>
-  </si>
-  <si>
-    <t>orderHandleInstruction</t>
-  </si>
-  <si>
-    <t>Total Cubic</t>
-  </si>
-  <si>
-    <t>totalCubic</t>
-  </si>
-  <si>
-    <t>Total Gross Weight</t>
-  </si>
-  <si>
-    <t>totalGrossWeight</t>
-  </si>
-  <si>
-    <t>Total Net Weight</t>
-  </si>
-  <si>
-    <t>totalNetWeight</t>
-  </si>
-  <si>
-    <t>Total Price</t>
-  </si>
-  <si>
-    <t>totalPrice</t>
-  </si>
-  <si>
-    <t>Total Line Count</t>
-  </si>
-  <si>
-    <t>totalLineCount</t>
-  </si>
-  <si>
-    <t>Cur LineNO</t>
-  </si>
-  <si>
-    <t>curLineNo</t>
-  </si>
-  <si>
-    <t>Parcel Mark</t>
-  </si>
-  <si>
-    <t>parcelMark</t>
-  </si>
-  <si>
-    <t>Parcel Consolidation</t>
-  </si>
-  <si>
-    <t>parcelConsolidation</t>
-  </si>
-  <si>
-    <t>Total SKU Count</t>
-  </si>
-  <si>
-    <t>totalSkuCount</t>
-  </si>
-  <si>
-    <t>Warehouse Transfer Flag</t>
-  </si>
-  <si>
-    <t>warehouseTransferFlag</t>
-  </si>
-  <si>
-    <t>ERP Cancel Reason</t>
-  </si>
-  <si>
-    <t>erpCancelReason</t>
-  </si>
-  <si>
-    <t>Express Platform</t>
-  </si>
-  <si>
-    <t>expressPlatform</t>
-  </si>
-  <si>
-    <t>OCP NO</t>
-  </si>
-  <si>
-    <t>ocpNo</t>
-  </si>
-  <si>
-    <t>VehicleNO</t>
-  </si>
-  <si>
-    <t>vehicleNo</t>
-  </si>
-  <si>
-    <t>Vehicle Type</t>
-  </si>
-  <si>
-    <t>vehicleType</t>
-  </si>
-  <si>
-    <t>Driver</t>
-  </si>
-  <si>
-    <t>driver</t>
-  </si>
-  <si>
-    <t>Split Flag</t>
-  </si>
-  <si>
-    <t>splitFlag</t>
-  </si>
-  <si>
-    <t>Order Source</t>
-  </si>
-  <si>
-    <t>orderSource</t>
-  </si>
-  <si>
-    <t>LOC Group1 List</t>
-  </si>
-  <si>
-    <t>locGroup1List</t>
-  </si>
-  <si>
-    <t>LOC Group2 List</t>
-  </si>
-  <si>
-    <t>locGroup2List</t>
-  </si>
-  <si>
-    <t>Shipment Count</t>
-  </si>
-  <si>
-    <t>shipmentCount</t>
-  </si>
-  <si>
-    <t>Wave Rule</t>
-  </si>
-  <si>
-    <t>waveRule</t>
-  </si>
-  <si>
-    <t>Reverse Order NO</t>
-  </si>
-  <si>
-    <t>reverseOrderno</t>
-  </si>
-  <si>
-    <t>Shop</t>
-  </si>
-  <si>
-    <t>shop</t>
-  </si>
-  <si>
-    <t>Replenish Group ID</t>
-  </si>
-  <si>
-    <t>rpGroupId</t>
-  </si>
-  <si>
-    <t>Total QTY</t>
-  </si>
-  <si>
-    <t>totalQty</t>
-  </si>
-  <si>
     <t>Note Text</t>
   </si>
   <si>
@@ -1135,6 +1268,12 @@
     <t>udf06</t>
   </si>
   <si>
+    <t>Task Flag</t>
+  </si>
+  <si>
+    <t>taskFlag</t>
+  </si>
+  <si>
     <t>D.warehouseId</t>
   </si>
   <si>
@@ -1369,55 +1508,55 @@
     <t>D.price</t>
   </si>
   <si>
-    <t>DEDI01</t>
+    <t>DEDI1</t>
   </si>
   <si>
     <t>D.dedi01</t>
   </si>
   <si>
-    <t>DEDI02</t>
+    <t>DEDI2</t>
   </si>
   <si>
     <t>D.dedi02</t>
   </si>
   <si>
-    <t>DEDI03</t>
+    <t>DEDI3</t>
   </si>
   <si>
     <t>D.dedi03</t>
   </si>
   <si>
-    <t>DEDI04</t>
+    <t>DEDI4</t>
   </si>
   <si>
     <t>D.dedi04</t>
   </si>
   <si>
-    <t>DEDI05</t>
+    <t>DEDI5</t>
   </si>
   <si>
     <t>D.dedi05</t>
   </si>
   <si>
-    <t>DEDI06</t>
+    <t>DEDI6</t>
   </si>
   <si>
     <t>D.dedi06</t>
   </si>
   <si>
-    <t>DEDI07</t>
+    <t>DEDI7</t>
   </si>
   <si>
     <t>D.dedi07</t>
   </si>
   <si>
-    <t>DEDI08</t>
+    <t>DEDI8</t>
   </si>
   <si>
     <t>D.dedi08</t>
   </si>
   <si>
-    <t>DEDI09</t>
+    <t>DEDI9</t>
   </si>
   <si>
     <t>D.dedi09</t>
@@ -1489,259 +1628,232 @@
     <t>D.dedi20</t>
   </si>
   <si>
+    <t>原產品名</t>
+  </si>
+  <si>
+    <t>D.originalSku</t>
+  </si>
+  <si>
+    <t>Kit ReferenceNO</t>
+  </si>
+  <si>
+    <t>D.kitReferenceNo</t>
+  </si>
+  <si>
+    <t>Order Line ReferenceNO</t>
+  </si>
+  <si>
+    <t>D.orderLineReferenceNo</t>
+  </si>
+  <si>
+    <t>Kit SKU</t>
+  </si>
+  <si>
+    <t>D.kitSku</t>
+  </si>
+  <si>
+    <t>D.erpCancelFlag</t>
+  </si>
+  <si>
+    <t>D.zoneGroup</t>
+  </si>
+  <si>
+    <t>LOC Group1</t>
+  </si>
+  <si>
+    <t>D.locGroup1</t>
+  </si>
+  <si>
+    <t>LOC Group2</t>
+  </si>
+  <si>
+    <t>D.locGroup2</t>
+  </si>
+  <si>
+    <t>Commingle SKU</t>
+  </si>
+  <si>
+    <t>D.commingleSku</t>
+  </si>
+  <si>
+    <t>One Step Allocation</t>
+  </si>
+  <si>
+    <t>D.oneStepAllocation</t>
+  </si>
+  <si>
+    <t>Order LOT Control</t>
+  </si>
+  <si>
+    <t>D.orderLotControl</t>
+  </si>
+  <si>
+    <t>Full Case LOT Control</t>
+  </si>
+  <si>
+    <t>D.fullCaseLotControl</t>
+  </si>
+  <si>
+    <t>Piece LOT Control</t>
+  </si>
+  <si>
+    <t>D.pieceLotControl</t>
+  </si>
+  <si>
+    <t>Reference LineNO</t>
+  </si>
+  <si>
+    <t>D.referenceLineNo</t>
+  </si>
+  <si>
+    <t>D.salesOrderNo</t>
+  </si>
+  <si>
+    <t>Sales Order LineNO</t>
+  </si>
+  <si>
+    <t>D.salesOrderLineNo</t>
+  </si>
+  <si>
+    <t>QTY Released</t>
+  </si>
+  <si>
+    <t>D.qtyReleased</t>
+  </si>
+  <si>
+    <t>Free Pick Gift</t>
+  </si>
+  <si>
+    <t>D.freePickGift</t>
+  </si>
+  <si>
+    <t>Rule3 Flag</t>
+  </si>
+  <si>
+    <t>D.rule3Flag</t>
+  </si>
+  <si>
+    <t>Allocation Where Sql</t>
+  </si>
+  <si>
+    <t>D.allocationWhereSql</t>
+  </si>
+  <si>
+    <t>D.noteText</t>
+  </si>
+  <si>
+    <t>D.udf01</t>
+  </si>
+  <si>
+    <t>D.udf02</t>
+  </si>
+  <si>
+    <t>D.udf03</t>
+  </si>
+  <si>
+    <t>D.udf04</t>
+  </si>
+  <si>
+    <t>D.udf05</t>
+  </si>
+  <si>
+    <t>D.udf06</t>
+  </si>
+  <si>
+    <t>LOTATT13</t>
+  </si>
+  <si>
+    <t>D.lotAtt13</t>
+  </si>
+  <si>
+    <t>LOTATT14</t>
+  </si>
+  <si>
+    <t>D.lotAtt14</t>
+  </si>
+  <si>
+    <t>LOTATT15</t>
+  </si>
+  <si>
+    <t>D.lotAtt15</t>
+  </si>
+  <si>
+    <t>LOTATT16</t>
+  </si>
+  <si>
+    <t>D.lotAtt16</t>
+  </si>
+  <si>
+    <t>LOTATT17</t>
+  </si>
+  <si>
+    <t>D.lotAtt17</t>
+  </si>
+  <si>
+    <t>LOTATT18</t>
+  </si>
+  <si>
+    <t>D.lotAtt18</t>
+  </si>
+  <si>
+    <t>LOTATT19</t>
+  </si>
+  <si>
+    <t>D.lotAtt19</t>
+  </si>
+  <si>
+    <t>LOTATT20</t>
+  </si>
+  <si>
+    <t>D.lotAtt20</t>
+  </si>
+  <si>
+    <t>LOTATT21</t>
+  </si>
+  <si>
+    <t>D.lotAtt21</t>
+  </si>
+  <si>
+    <t>LOTATT22</t>
+  </si>
+  <si>
+    <t>D.lotAtt22</t>
+  </si>
+  <si>
+    <t>LOTATT23</t>
+  </si>
+  <si>
+    <t>D.lotAtt23</t>
+  </si>
+  <si>
+    <t>LOTATT24</t>
+  </si>
+  <si>
+    <t>D.lotAtt24</t>
+  </si>
+  <si>
+    <t>MUID</t>
+  </si>
+  <si>
+    <t>D.muid</t>
+  </si>
+  <si>
+    <t>Pick Instruction</t>
+  </si>
+  <si>
+    <t>D.pickInstruction</t>
+  </si>
+  <si>
     <t>Alternative SKU</t>
   </si>
   <si>
     <t>D.alternativeSku</t>
   </si>
   <si>
-    <t>Kit ReferenceNO</t>
-  </si>
-  <si>
-    <t>D.kitReferenceNo</t>
-  </si>
-  <si>
-    <t>Order Line ReferenceNO</t>
-  </si>
-  <si>
-    <t>D.orderLineReferenceNo</t>
-  </si>
-  <si>
-    <t>Kit SKU</t>
-  </si>
-  <si>
-    <t>D.kitSku</t>
-  </si>
-  <si>
-    <t>D.erpCancelFlag</t>
-  </si>
-  <si>
-    <t>D.zoneGroup</t>
-  </si>
-  <si>
-    <t>LOC Group1</t>
-  </si>
-  <si>
-    <t>D.locGroup1</t>
-  </si>
-  <si>
-    <t>LOC Group2</t>
-  </si>
-  <si>
-    <t>D.locGroup2</t>
-  </si>
-  <si>
-    <t>Commingle SKU</t>
-  </si>
-  <si>
-    <t>D.commingleSku</t>
-  </si>
-  <si>
-    <t>One Step Allocation</t>
-  </si>
-  <si>
-    <t>D.oneStepAllocation</t>
-  </si>
-  <si>
-    <t>Order LOT Control</t>
-  </si>
-  <si>
-    <t>D.orderLotControl</t>
-  </si>
-  <si>
-    <t>Full Case LOT Control</t>
-  </si>
-  <si>
-    <t>D.fullCaseLotControl</t>
-  </si>
-  <si>
-    <t>Piece LOT Control</t>
-  </si>
-  <si>
-    <t>D.pieceLotControl</t>
-  </si>
-  <si>
-    <t>Reference LineNO</t>
-  </si>
-  <si>
-    <t>D.referenceLineNo</t>
-  </si>
-  <si>
-    <t>D.salesOrderNo</t>
-  </si>
-  <si>
-    <t>Sales Order LineNO</t>
-  </si>
-  <si>
-    <t>D.salesOrderLineNo</t>
-  </si>
-  <si>
-    <t>QTY Released</t>
-  </si>
-  <si>
-    <t>D.qtyReleased</t>
-  </si>
-  <si>
-    <t>Free Pick Gift</t>
-  </si>
-  <si>
-    <t>D.freePickGift</t>
-  </si>
-  <si>
-    <t>Rule3 Flag</t>
-  </si>
-  <si>
-    <t>D.rule3Flag</t>
-  </si>
-  <si>
-    <t>Allocation Where Sql</t>
-  </si>
-  <si>
-    <t>D.allocationWhereSql</t>
-  </si>
-  <si>
-    <t>D.noteText</t>
-  </si>
-  <si>
-    <t>D.udf01</t>
-  </si>
-  <si>
-    <t>D.udf02</t>
-  </si>
-  <si>
-    <t>D.udf03</t>
-  </si>
-  <si>
-    <t>D.udf04</t>
-  </si>
-  <si>
-    <t>D.udf05</t>
-  </si>
-  <si>
-    <t>D.udf06</t>
-  </si>
-  <si>
-    <t>LOTATT13</t>
-  </si>
-  <si>
-    <t>D.lotAtt13</t>
-  </si>
-  <si>
-    <t>LOTATT14</t>
-  </si>
-  <si>
-    <t>D.lotAtt14</t>
-  </si>
-  <si>
-    <t>LOTATT15</t>
-  </si>
-  <si>
-    <t>D.lotAtt15</t>
-  </si>
-  <si>
-    <t>LOTATT16</t>
-  </si>
-  <si>
-    <t>D.lotAtt16</t>
-  </si>
-  <si>
-    <t>LOTATT17</t>
-  </si>
-  <si>
-    <t>D.lotAtt17</t>
-  </si>
-  <si>
-    <t>LOTATT18</t>
-  </si>
-  <si>
-    <t>D.lotAtt18</t>
-  </si>
-  <si>
-    <t>LOTATT19</t>
-  </si>
-  <si>
-    <t>D.lotAtt19</t>
-  </si>
-  <si>
-    <t>LOTATT20</t>
-  </si>
-  <si>
-    <t>D.lotAtt20</t>
-  </si>
-  <si>
-    <t>LOTATT21</t>
-  </si>
-  <si>
-    <t>D.lotAtt21</t>
-  </si>
-  <si>
-    <t>LOTATT22</t>
-  </si>
-  <si>
-    <t>D.lotAtt22</t>
-  </si>
-  <si>
-    <t>LOTATT23</t>
-  </si>
-  <si>
-    <t>D.lotAtt23</t>
-  </si>
-  <si>
-    <t>LOTATT24</t>
-  </si>
-  <si>
-    <t>D.lotAtt24</t>
-  </si>
-  <si>
-    <t>MUID</t>
-  </si>
-  <si>
-    <t>D.muid</t>
-  </si>
-  <si>
-    <t>Pick Instruction</t>
-  </si>
-  <si>
-    <t>D.pickInstruction</t>
-  </si>
-  <si>
-    <t>Ship to</t>
-  </si>
-  <si>
-    <t>Warehouse ID Item</t>
-  </si>
-  <si>
-    <t>Customer ID Item</t>
-  </si>
-  <si>
-    <t>Erp Cancel Flag Item</t>
-  </si>
-  <si>
-    <t>Zone Group Item</t>
-  </si>
-  <si>
-    <t>Sales OrderNO Item</t>
-  </si>
-  <si>
-    <t>Note Text Item</t>
-  </si>
-  <si>
-    <t>UDF01 Item</t>
-  </si>
-  <si>
-    <t>UDF02 Item</t>
-  </si>
-  <si>
-    <t>UDF03 Item</t>
-  </si>
-  <si>
-    <t>UDF04 Item</t>
-  </si>
-  <si>
-    <t>UDF05 Item</t>
-  </si>
-  <si>
-    <t>UDF06 Item</t>
+    <t>Reference Line No</t>
+  </si>
+  <si>
+    <t>D.refLineNo</t>
   </si>
 </sst>
 </file>
@@ -1796,7 +1908,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="290">
+  <cellXfs count="292">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1941,7 +2053,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1975,14 +2086,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2067,6 +2179,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2404,306 +2518,308 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:KA2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:KC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="JA1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="JG8" sqref="JG8"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.140625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14" style="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.28515625" style="25" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.28515625" style="26" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.7109375" style="27" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18" style="28" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.7109375" style="30" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.28515625" style="32" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.7109375" style="33" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.7109375" style="34" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.85546875" style="35" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.28515625" style="36" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.28515625" style="37" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.28515625" style="39" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.28515625" style="40" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.42578125" style="41" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="13.42578125" style="42" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.42578125" style="43" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="14.85546875" style="44" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.140625" style="45" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="9.7109375" style="46" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.85546875" style="47" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.85546875" style="48" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="10.42578125" style="49" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="10.85546875" style="50" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.85546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.42578125" style="52" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="19.85546875" style="53" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="14.85546875" style="54" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="20.28515625" style="55" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="14.140625" style="56" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="5.28515625" style="57" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="6.28515625" style="58" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="11.7109375" style="59" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="15.7109375" style="60" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="17.5703125" style="61" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="16.28515625" style="62" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="9.28515625" style="63" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="12.7109375" style="64" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="15.7109375" style="65" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="15.7109375" style="66" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="15.7109375" style="67" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="15.7109375" style="68" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="12.85546875" style="69" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="13.85546875" style="70" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="10.85546875" style="71" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="15.28515625" style="72" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="14.5703125" style="73" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="10.140625" style="74" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="14.28515625" style="75" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="12.28515625" style="76" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="10.85546875" style="77" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="11.28515625" style="78" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="11.28515625" style="79" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="12.5703125" style="80" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="16.42578125" style="81" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="19.42578125" style="82" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="19.42578125" style="83" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="19.42578125" style="84" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="19.42578125" style="85" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="16.5703125" style="86" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="17.5703125" style="87" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="14.5703125" style="88" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="19" style="89" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="18.28515625" style="90" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="13.85546875" style="91" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="18" style="92" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="16" style="93" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="14.5703125" style="94" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="15" style="95" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="15" style="96" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="7.140625" style="97" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="7.140625" style="98" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="7.140625" style="99" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="7.140625" style="100" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="7.140625" style="101" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="7.140625" style="102" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="7.140625" style="103" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="7.140625" style="104" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="7.140625" style="105" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="7.140625" style="106" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="7.140625" style="107" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="7.140625" style="108" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="7.140625" style="109" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="7.140625" style="110" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="7.140625" style="111" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="7.140625" style="112" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="7.140625" style="113" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="7.140625" style="114" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="7.140625" style="115" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="7.140625" style="116" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="12.7109375" style="117" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="14.7109375" style="118" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="14.7109375" style="119" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="13.7109375" style="120" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="13.7109375" style="121" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="16.85546875" style="122" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="13.85546875" style="123" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="14.7109375" style="124" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="18" style="125" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="13.85546875" style="126" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="14.7109375" style="127" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="18" style="128" bestFit="1" customWidth="1"/>
-    <col min="127" max="127" width="11" style="129" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="14.7109375" style="130" bestFit="1" customWidth="1"/>
-    <col min="129" max="129" width="12.28515625" style="131" bestFit="1" customWidth="1"/>
-    <col min="130" max="130" width="14.28515625" style="132" bestFit="1" customWidth="1"/>
-    <col min="131" max="131" width="19" style="133" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="11.7109375" style="134" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="7.85546875" style="135" bestFit="1" customWidth="1"/>
-    <col min="134" max="134" width="8.28515625" style="136" bestFit="1" customWidth="1"/>
-    <col min="135" max="135" width="14.28515625" style="137" bestFit="1" customWidth="1"/>
-    <col min="136" max="136" width="15.28515625" style="138" bestFit="1" customWidth="1"/>
-    <col min="137" max="137" width="16.7109375" style="139" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="14.42578125" style="140" bestFit="1" customWidth="1"/>
-    <col min="139" max="139" width="18.5703125" style="141" bestFit="1" customWidth="1"/>
-    <col min="140" max="140" width="13.42578125" style="142" bestFit="1" customWidth="1"/>
-    <col min="141" max="141" width="11.28515625" style="143" bestFit="1" customWidth="1"/>
-    <col min="142" max="142" width="16.85546875" style="144" bestFit="1" customWidth="1"/>
-    <col min="143" max="143" width="9.85546875" style="145" bestFit="1" customWidth="1"/>
-    <col min="144" max="144" width="13.5703125" style="146" bestFit="1" customWidth="1"/>
-    <col min="145" max="145" width="14.85546875" style="147" bestFit="1" customWidth="1"/>
-    <col min="146" max="146" width="11.28515625" style="148" bestFit="1" customWidth="1"/>
-    <col min="147" max="147" width="15.85546875" style="149" bestFit="1" customWidth="1"/>
-    <col min="148" max="148" width="8.85546875" style="150" bestFit="1" customWidth="1"/>
-    <col min="149" max="149" width="12.7109375" style="151" bestFit="1" customWidth="1"/>
-    <col min="150" max="150" width="9.140625" style="152" bestFit="1" customWidth="1"/>
-    <col min="151" max="151" width="15" style="153" bestFit="1" customWidth="1"/>
-    <col min="152" max="152" width="18" style="154" bestFit="1" customWidth="1"/>
-    <col min="153" max="153" width="23.28515625" style="155" bestFit="1" customWidth="1"/>
-    <col min="154" max="154" width="10.7109375" style="156" bestFit="1" customWidth="1"/>
-    <col min="155" max="155" width="17.85546875" style="157" bestFit="1" customWidth="1"/>
-    <col min="156" max="156" width="16.140625" style="158" bestFit="1" customWidth="1"/>
-    <col min="157" max="157" width="10.28515625" style="159" bestFit="1" customWidth="1"/>
-    <col min="158" max="158" width="15.42578125" style="160" bestFit="1" customWidth="1"/>
-    <col min="159" max="159" width="11" style="161" bestFit="1" customWidth="1"/>
-    <col min="160" max="160" width="11.28515625" style="162" bestFit="1" customWidth="1"/>
-    <col min="161" max="161" width="19.42578125" style="163" bestFit="1" customWidth="1"/>
-    <col min="162" max="162" width="15.140625" style="164" bestFit="1" customWidth="1"/>
-    <col min="163" max="163" width="23.28515625" style="165" bestFit="1" customWidth="1"/>
-    <col min="164" max="164" width="17.7109375" style="166" bestFit="1" customWidth="1"/>
-    <col min="165" max="165" width="16" style="167" bestFit="1" customWidth="1"/>
-    <col min="166" max="166" width="8" style="168" bestFit="1" customWidth="1"/>
-    <col min="167" max="167" width="10.5703125" style="169" bestFit="1" customWidth="1"/>
-    <col min="168" max="168" width="12.42578125" style="170" bestFit="1" customWidth="1"/>
-    <col min="169" max="169" width="6.42578125" style="171" bestFit="1" customWidth="1"/>
-    <col min="170" max="170" width="9" style="172" bestFit="1" customWidth="1"/>
-    <col min="171" max="171" width="12.5703125" style="173" bestFit="1" customWidth="1"/>
-    <col min="172" max="172" width="14.85546875" style="174" bestFit="1" customWidth="1"/>
-    <col min="173" max="173" width="14.85546875" style="175" bestFit="1" customWidth="1"/>
-    <col min="174" max="174" width="15.42578125" style="176" bestFit="1" customWidth="1"/>
-    <col min="175" max="175" width="10.42578125" style="177" bestFit="1" customWidth="1"/>
-    <col min="176" max="176" width="17.28515625" style="178" bestFit="1" customWidth="1"/>
-    <col min="177" max="177" width="5.42578125" style="179" bestFit="1" customWidth="1"/>
-    <col min="178" max="178" width="18.28515625" style="180" bestFit="1" customWidth="1"/>
-    <col min="179" max="179" width="9.28515625" style="181" bestFit="1" customWidth="1"/>
-    <col min="180" max="180" width="9.7109375" style="182" bestFit="1" customWidth="1"/>
-    <col min="181" max="181" width="6.5703125" style="183" bestFit="1" customWidth="1"/>
-    <col min="182" max="182" width="6.5703125" style="184" bestFit="1" customWidth="1"/>
-    <col min="183" max="183" width="6.5703125" style="185" bestFit="1" customWidth="1"/>
-    <col min="184" max="184" width="6.5703125" style="186" bestFit="1" customWidth="1"/>
-    <col min="185" max="185" width="6.5703125" style="187" bestFit="1" customWidth="1"/>
-    <col min="186" max="186" width="6.5703125" style="188" bestFit="1" customWidth="1"/>
-    <col min="187" max="187" width="18.28515625" style="189" bestFit="1" customWidth="1"/>
-    <col min="188" max="188" width="14.140625" style="190" bestFit="1" customWidth="1"/>
-    <col min="189" max="189" width="16.5703125" style="191" bestFit="1" customWidth="1"/>
-    <col min="190" max="190" width="5.85546875" style="192" bestFit="1" customWidth="1"/>
-    <col min="191" max="191" width="11.7109375" style="193" bestFit="1" customWidth="1"/>
-    <col min="192" max="192" width="9.5703125" style="194" bestFit="1" customWidth="1"/>
-    <col min="193" max="193" width="10" style="195" bestFit="1" customWidth="1"/>
-    <col min="194" max="194" width="10" style="196" bestFit="1" customWidth="1"/>
-    <col min="195" max="195" width="10" style="197" bestFit="1" customWidth="1"/>
-    <col min="196" max="196" width="10" style="198" bestFit="1" customWidth="1"/>
-    <col min="197" max="197" width="10" style="199" bestFit="1" customWidth="1"/>
-    <col min="198" max="198" width="10" style="200" bestFit="1" customWidth="1"/>
-    <col min="199" max="199" width="10" style="201" bestFit="1" customWidth="1"/>
-    <col min="200" max="200" width="10" style="202" bestFit="1" customWidth="1"/>
-    <col min="201" max="201" width="10" style="203" bestFit="1" customWidth="1"/>
-    <col min="202" max="202" width="10" style="204" bestFit="1" customWidth="1"/>
-    <col min="203" max="203" width="10" style="205" bestFit="1" customWidth="1"/>
-    <col min="204" max="204" width="10" style="206" bestFit="1" customWidth="1"/>
-    <col min="205" max="205" width="10.85546875" style="207" bestFit="1" customWidth="1"/>
-    <col min="206" max="206" width="10" style="208" bestFit="1" customWidth="1"/>
-    <col min="207" max="207" width="9" style="209" bestFit="1" customWidth="1"/>
-    <col min="208" max="208" width="13.28515625" style="210" bestFit="1" customWidth="1"/>
-    <col min="209" max="209" width="18" style="211" bestFit="1" customWidth="1"/>
-    <col min="210" max="210" width="14.28515625" style="212" bestFit="1" customWidth="1"/>
-    <col min="211" max="211" width="11.5703125" style="213" bestFit="1" customWidth="1"/>
-    <col min="212" max="212" width="13.140625" style="214" bestFit="1"/>
-    <col min="213" max="213" width="8.5703125" style="215" bestFit="1" customWidth="1"/>
-    <col min="214" max="214" width="11" style="216" bestFit="1" customWidth="1"/>
-    <col min="215" max="215" width="18.5703125" style="217" bestFit="1" customWidth="1"/>
-    <col min="216" max="216" width="23.28515625" style="218" bestFit="1" customWidth="1"/>
-    <col min="217" max="217" width="19.5703125" style="219" bestFit="1" customWidth="1"/>
-    <col min="218" max="218" width="16.85546875" style="220" bestFit="1" customWidth="1"/>
-    <col min="219" max="219" width="18.42578125" style="221" bestFit="1" customWidth="1"/>
-    <col min="220" max="220" width="11.7109375" style="222" bestFit="1" customWidth="1"/>
-    <col min="221" max="221" width="19.5703125" style="223" bestFit="1" customWidth="1"/>
-    <col min="222" max="222" width="15.7109375" style="224" bestFit="1" customWidth="1"/>
-    <col min="223" max="223" width="14" style="225" bestFit="1" customWidth="1"/>
-    <col min="224" max="224" width="12.28515625" style="226" bestFit="1" customWidth="1"/>
-    <col min="225" max="225" width="7.42578125" style="227" bestFit="1" customWidth="1"/>
-    <col min="226" max="226" width="7.28515625" style="228" bestFit="1" customWidth="1"/>
-    <col min="227" max="227" width="8.85546875" style="229" bestFit="1" customWidth="1"/>
-    <col min="228" max="228" width="8.85546875" style="230" bestFit="1" customWidth="1"/>
-    <col min="229" max="229" width="8.85546875" style="231" bestFit="1" customWidth="1"/>
-    <col min="230" max="230" width="8.85546875" style="232" bestFit="1" customWidth="1"/>
-    <col min="231" max="231" width="8.85546875" style="233" bestFit="1" customWidth="1"/>
-    <col min="232" max="232" width="8.85546875" style="234" bestFit="1" customWidth="1"/>
-    <col min="233" max="233" width="8.85546875" style="235" bestFit="1" customWidth="1"/>
-    <col min="234" max="234" width="8.85546875" style="236" bestFit="1" customWidth="1"/>
-    <col min="235" max="235" width="8.85546875" style="237" bestFit="1" customWidth="1"/>
-    <col min="236" max="236" width="8.85546875" style="238" bestFit="1" customWidth="1"/>
-    <col min="237" max="237" width="8.85546875" style="239" bestFit="1" customWidth="1"/>
-    <col min="238" max="238" width="8.85546875" style="240" bestFit="1" customWidth="1"/>
-    <col min="239" max="239" width="8.85546875" style="241" bestFit="1" customWidth="1"/>
-    <col min="240" max="240" width="8.85546875" style="242" bestFit="1" customWidth="1"/>
-    <col min="241" max="241" width="8.85546875" style="243" bestFit="1" customWidth="1"/>
-    <col min="242" max="242" width="8.85546875" style="244" bestFit="1" customWidth="1"/>
-    <col min="243" max="243" width="8.85546875" style="245" bestFit="1" customWidth="1"/>
-    <col min="244" max="244" width="8.85546875" style="246" bestFit="1" customWidth="1"/>
-    <col min="245" max="245" width="8.85546875" style="247" bestFit="1" customWidth="1"/>
-    <col min="246" max="246" width="8.85546875" style="248" bestFit="1" customWidth="1"/>
-    <col min="247" max="247" width="15.85546875" style="249" bestFit="1" customWidth="1"/>
-    <col min="248" max="248" width="17" style="250" bestFit="1" customWidth="1"/>
-    <col min="249" max="249" width="23.5703125" style="251" bestFit="1" customWidth="1"/>
-    <col min="250" max="250" width="8.28515625" style="252" bestFit="1" customWidth="1"/>
-    <col min="251" max="251" width="15.42578125" style="253" bestFit="1" customWidth="1"/>
-    <col min="252" max="252" width="12.5703125" style="254" bestFit="1" customWidth="1"/>
-    <col min="253" max="253" width="11.85546875" style="255" bestFit="1" customWidth="1"/>
-    <col min="254" max="254" width="11.85546875" style="256" bestFit="1" customWidth="1"/>
-    <col min="255" max="255" width="16" style="257" bestFit="1" customWidth="1"/>
-    <col min="256" max="256" width="19.5703125" style="258" bestFit="1" customWidth="1"/>
-    <col min="257" max="257" width="17.28515625" style="259" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="19.85546875" style="260" bestFit="1" customWidth="1"/>
-    <col min="259" max="259" width="17.28515625" style="261" bestFit="1" customWidth="1"/>
-    <col min="260" max="260" width="18.140625" style="262" bestFit="1" customWidth="1"/>
-    <col min="261" max="261" width="15.140625" style="263" bestFit="1" customWidth="1"/>
-    <col min="262" max="262" width="19" style="264" bestFit="1" customWidth="1"/>
-    <col min="263" max="263" width="14" style="265" bestFit="1" customWidth="1"/>
-    <col min="264" max="264" width="13.5703125" style="266" bestFit="1" customWidth="1"/>
-    <col min="265" max="265" width="11" style="267" bestFit="1" customWidth="1"/>
-    <col min="266" max="266" width="20.5703125" style="268" bestFit="1" customWidth="1"/>
-    <col min="267" max="267" width="10.85546875" style="269" bestFit="1" customWidth="1"/>
-    <col min="268" max="268" width="7.85546875" style="270" bestFit="1" customWidth="1"/>
-    <col min="269" max="269" width="7.85546875" style="271" bestFit="1" customWidth="1"/>
-    <col min="270" max="270" width="7.85546875" style="272" bestFit="1" customWidth="1"/>
-    <col min="271" max="271" width="7.85546875" style="273" bestFit="1" customWidth="1"/>
-    <col min="272" max="272" width="7.85546875" style="274" bestFit="1" customWidth="1"/>
-    <col min="273" max="273" width="7.85546875" style="275" bestFit="1" customWidth="1"/>
-    <col min="274" max="274" width="10" style="276" bestFit="1" customWidth="1"/>
-    <col min="275" max="275" width="10" style="277" bestFit="1" customWidth="1"/>
-    <col min="276" max="276" width="10" style="278" bestFit="1" customWidth="1"/>
-    <col min="277" max="277" width="10" style="279" bestFit="1" customWidth="1"/>
-    <col min="278" max="278" width="10" style="280" bestFit="1" customWidth="1"/>
-    <col min="279" max="279" width="10" style="281" bestFit="1" customWidth="1"/>
-    <col min="280" max="280" width="10" style="282" bestFit="1" customWidth="1"/>
-    <col min="281" max="281" width="10" style="283" bestFit="1" customWidth="1"/>
-    <col min="282" max="282" width="10" style="284" bestFit="1" customWidth="1"/>
-    <col min="283" max="283" width="10" style="285" bestFit="1" customWidth="1"/>
-    <col min="284" max="284" width="10" style="286" bestFit="1" customWidth="1"/>
-    <col min="285" max="285" width="10" style="287" bestFit="1" customWidth="1"/>
-    <col min="286" max="286" width="7.42578125" style="288" bestFit="1" customWidth="1"/>
-    <col min="287" max="287" width="16.140625" style="289" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" style="3"/>
+    <col min="2" max="2" width="12" style="4"/>
+    <col min="3" max="3" width="12" style="5"/>
+    <col min="4" max="4" width="12" style="6"/>
+    <col min="5" max="5" width="12" style="7"/>
+    <col min="6" max="6" width="12" style="8"/>
+    <col min="7" max="7" width="12" style="9"/>
+    <col min="8" max="8" width="12" style="10"/>
+    <col min="9" max="9" width="12" style="11"/>
+    <col min="10" max="10" width="12" style="12"/>
+    <col min="11" max="11" width="12" style="13"/>
+    <col min="12" max="12" width="12" style="14"/>
+    <col min="13" max="13" width="12" style="15"/>
+    <col min="14" max="14" width="12" style="16"/>
+    <col min="15" max="15" width="12" style="17"/>
+    <col min="16" max="16" width="12" style="18"/>
+    <col min="17" max="17" width="12" style="19"/>
+    <col min="18" max="18" width="12" style="20"/>
+    <col min="19" max="19" width="12" style="21"/>
+    <col min="20" max="20" width="12" style="22"/>
+    <col min="21" max="21" width="12" style="23"/>
+    <col min="22" max="22" width="12" style="24"/>
+    <col min="23" max="23" width="12" style="25"/>
+    <col min="24" max="24" width="12" style="26"/>
+    <col min="25" max="25" width="12" style="27"/>
+    <col min="26" max="26" width="12" style="28"/>
+    <col min="27" max="27" width="12" style="29"/>
+    <col min="28" max="28" width="12" style="30"/>
+    <col min="29" max="29" width="12" style="31"/>
+    <col min="30" max="30" width="12" style="32"/>
+    <col min="31" max="31" width="12" style="33"/>
+    <col min="32" max="32" width="12" style="34"/>
+    <col min="33" max="33" width="12" style="35"/>
+    <col min="34" max="34" width="12" style="36"/>
+    <col min="35" max="35" width="12" style="37"/>
+    <col min="36" max="36" width="12" style="38"/>
+    <col min="37" max="37" width="12" style="39"/>
+    <col min="38" max="38" width="12" style="40"/>
+    <col min="39" max="39" width="12" style="41"/>
+    <col min="40" max="40" width="12" style="42"/>
+    <col min="41" max="41" width="12" style="43"/>
+    <col min="42" max="42" width="12" style="44"/>
+    <col min="43" max="43" width="12" style="45"/>
+    <col min="44" max="44" width="12" style="46"/>
+    <col min="45" max="45" width="12" style="47"/>
+    <col min="46" max="46" width="12" style="48"/>
+    <col min="47" max="47" width="12" style="49"/>
+    <col min="48" max="48" width="12" style="50"/>
+    <col min="49" max="49" width="12" style="51"/>
+    <col min="50" max="50" width="12" style="52"/>
+    <col min="51" max="51" width="12" style="53"/>
+    <col min="52" max="52" width="12" style="54"/>
+    <col min="53" max="53" width="12" style="55"/>
+    <col min="54" max="54" width="12" style="56"/>
+    <col min="55" max="55" width="12" style="57"/>
+    <col min="56" max="56" width="12" style="58"/>
+    <col min="57" max="57" width="12" style="59"/>
+    <col min="58" max="58" width="12" style="60"/>
+    <col min="59" max="59" width="12" style="61"/>
+    <col min="60" max="60" width="12" style="62"/>
+    <col min="61" max="61" width="12" style="63"/>
+    <col min="62" max="62" width="12" style="64"/>
+    <col min="63" max="63" width="12" style="65"/>
+    <col min="64" max="64" width="12" style="66"/>
+    <col min="65" max="65" width="12" style="67"/>
+    <col min="66" max="66" width="12" style="68"/>
+    <col min="67" max="67" width="12" style="69"/>
+    <col min="68" max="68" width="12" style="70"/>
+    <col min="69" max="69" width="12" style="71"/>
+    <col min="70" max="70" width="12" style="72"/>
+    <col min="71" max="71" width="12" style="73"/>
+    <col min="72" max="72" width="12" style="74"/>
+    <col min="73" max="73" width="12" style="75"/>
+    <col min="74" max="74" width="12" style="76"/>
+    <col min="75" max="75" width="12" style="77"/>
+    <col min="76" max="76" width="12" style="78"/>
+    <col min="77" max="77" width="12" style="79"/>
+    <col min="78" max="78" width="12" style="80"/>
+    <col min="79" max="79" width="12" style="81"/>
+    <col min="80" max="80" width="12" style="82"/>
+    <col min="81" max="81" width="12" style="83"/>
+    <col min="82" max="82" width="12" style="84"/>
+    <col min="83" max="83" width="12" style="85"/>
+    <col min="84" max="84" width="12" style="86"/>
+    <col min="85" max="85" width="12" style="87"/>
+    <col min="86" max="86" width="12" style="88"/>
+    <col min="87" max="87" width="12" style="89"/>
+    <col min="88" max="88" width="12" style="90"/>
+    <col min="89" max="89" width="12" style="91"/>
+    <col min="90" max="90" width="12" style="92"/>
+    <col min="91" max="91" width="12" style="93"/>
+    <col min="92" max="92" width="12" style="94"/>
+    <col min="93" max="93" width="12" style="95"/>
+    <col min="94" max="94" width="12" style="96"/>
+    <col min="95" max="95" width="12" style="97"/>
+    <col min="96" max="96" width="12" style="98"/>
+    <col min="97" max="97" width="12" style="99"/>
+    <col min="98" max="98" width="12" style="100"/>
+    <col min="99" max="99" width="12" style="101"/>
+    <col min="100" max="100" width="12" style="102"/>
+    <col min="101" max="101" width="12" style="103"/>
+    <col min="102" max="102" width="12" style="104"/>
+    <col min="103" max="103" width="12" style="105"/>
+    <col min="104" max="104" width="12" style="106"/>
+    <col min="105" max="105" width="12" style="107"/>
+    <col min="106" max="106" width="12" style="108"/>
+    <col min="107" max="107" width="12" style="109"/>
+    <col min="108" max="108" width="12" style="110"/>
+    <col min="109" max="109" width="12" style="111"/>
+    <col min="110" max="110" width="12" style="112"/>
+    <col min="111" max="111" width="12" style="113"/>
+    <col min="112" max="112" width="12" style="114"/>
+    <col min="113" max="113" width="12" style="115"/>
+    <col min="114" max="114" width="12" style="116"/>
+    <col min="115" max="115" width="12" style="117"/>
+    <col min="116" max="116" width="12" style="118"/>
+    <col min="117" max="117" width="12" style="119"/>
+    <col min="118" max="118" width="12" style="120"/>
+    <col min="119" max="119" width="12" style="121"/>
+    <col min="120" max="120" width="12" style="122"/>
+    <col min="121" max="121" width="12" style="123"/>
+    <col min="122" max="122" width="12" style="124"/>
+    <col min="123" max="123" width="12" style="125"/>
+    <col min="124" max="124" width="12" style="126"/>
+    <col min="125" max="125" width="12" style="127"/>
+    <col min="126" max="126" width="12" style="128"/>
+    <col min="127" max="127" width="12" style="129"/>
+    <col min="128" max="128" width="12" style="130"/>
+    <col min="129" max="129" width="12" style="131"/>
+    <col min="130" max="130" width="12" style="132"/>
+    <col min="131" max="131" width="12" style="133"/>
+    <col min="132" max="132" width="12" style="134"/>
+    <col min="133" max="133" width="12" style="135"/>
+    <col min="134" max="134" width="12" style="136"/>
+    <col min="135" max="135" width="12" style="137"/>
+    <col min="136" max="136" width="12" style="138"/>
+    <col min="137" max="137" width="12" style="139"/>
+    <col min="138" max="138" width="12" style="140"/>
+    <col min="139" max="139" width="12" style="141"/>
+    <col min="140" max="140" width="12" style="142"/>
+    <col min="141" max="141" width="12" style="143"/>
+    <col min="142" max="142" width="12" style="144"/>
+    <col min="143" max="143" width="12" style="145"/>
+    <col min="144" max="144" width="12" style="146"/>
+    <col min="145" max="145" width="12" style="147"/>
+    <col min="146" max="146" width="12" style="148"/>
+    <col min="147" max="147" width="12" style="149"/>
+    <col min="148" max="148" width="12" style="150"/>
+    <col min="149" max="149" width="12" style="151"/>
+    <col min="150" max="150" width="12" style="152"/>
+    <col min="151" max="151" width="12" style="153"/>
+    <col min="152" max="152" width="12" style="154"/>
+    <col min="153" max="153" width="12" style="155"/>
+    <col min="154" max="154" width="12" style="156"/>
+    <col min="155" max="155" width="12" style="157"/>
+    <col min="156" max="156" width="12" style="158"/>
+    <col min="157" max="157" width="12" style="159"/>
+    <col min="158" max="158" width="12" style="160"/>
+    <col min="159" max="159" width="12" style="161"/>
+    <col min="160" max="160" width="12" style="162"/>
+    <col min="161" max="161" width="12" style="163"/>
+    <col min="162" max="162" width="12" style="164"/>
+    <col min="163" max="163" width="12" style="165"/>
+    <col min="164" max="164" width="12" style="166"/>
+    <col min="165" max="165" width="12" style="167"/>
+    <col min="166" max="166" width="12" style="168"/>
+    <col min="167" max="167" width="12" style="169"/>
+    <col min="168" max="168" width="12" style="170"/>
+    <col min="169" max="169" width="12" style="171"/>
+    <col min="170" max="170" width="12" style="172"/>
+    <col min="171" max="171" width="12" style="173"/>
+    <col min="172" max="172" width="12" style="174"/>
+    <col min="173" max="173" width="12" style="175"/>
+    <col min="174" max="174" width="12" style="176"/>
+    <col min="175" max="175" width="12" style="177"/>
+    <col min="176" max="176" width="12" style="178"/>
+    <col min="177" max="177" width="12" style="179"/>
+    <col min="178" max="178" width="12" style="180"/>
+    <col min="179" max="179" width="12" style="181"/>
+    <col min="180" max="180" width="12" style="182"/>
+    <col min="181" max="181" width="12" style="183"/>
+    <col min="182" max="182" width="12" style="184"/>
+    <col min="183" max="183" width="12" style="185"/>
+    <col min="184" max="184" width="12" style="186"/>
+    <col min="185" max="185" width="12" style="187"/>
+    <col min="186" max="186" width="12" style="188"/>
+    <col min="187" max="187" width="12" style="189"/>
+    <col min="188" max="188" width="12" style="190"/>
+    <col min="189" max="189" width="12" style="191"/>
+    <col min="190" max="190" width="12" style="192"/>
+    <col min="191" max="191" width="12" style="193"/>
+    <col min="192" max="192" width="12" style="194"/>
+    <col min="193" max="193" width="12" style="195"/>
+    <col min="194" max="194" width="12" style="196"/>
+    <col min="195" max="195" width="12" style="197"/>
+    <col min="196" max="196" width="12" style="198"/>
+    <col min="197" max="197" width="12" style="199"/>
+    <col min="198" max="198" width="12" style="200"/>
+    <col min="199" max="199" width="12" style="201"/>
+    <col min="200" max="200" width="12" style="202"/>
+    <col min="201" max="201" width="12" style="203"/>
+    <col min="202" max="202" width="12" style="204"/>
+    <col min="203" max="203" width="12" style="205"/>
+    <col min="204" max="204" width="12" style="206"/>
+    <col min="205" max="205" width="12" style="207"/>
+    <col min="206" max="206" width="12" style="208"/>
+    <col min="207" max="207" width="12" style="209"/>
+    <col min="208" max="208" width="12" style="210"/>
+    <col min="209" max="209" width="12" style="211"/>
+    <col min="210" max="210" width="12" style="212"/>
+    <col min="211" max="211" width="12" style="213"/>
+    <col min="212" max="212" width="12" style="214"/>
+    <col min="213" max="213" width="12" style="215"/>
+    <col min="214" max="214" width="12" style="216"/>
+    <col min="215" max="215" width="12" style="217"/>
+    <col min="216" max="216" width="12" style="218"/>
+    <col min="217" max="217" width="12" style="219"/>
+    <col min="218" max="218" width="12" style="220"/>
+    <col min="219" max="219" width="12" style="221"/>
+    <col min="220" max="220" width="12" style="222"/>
+    <col min="221" max="221" width="12" style="223"/>
+    <col min="222" max="222" width="12" style="224"/>
+    <col min="223" max="223" width="12" style="225"/>
+    <col min="224" max="224" width="12" style="226"/>
+    <col min="225" max="225" width="12" style="227"/>
+    <col min="226" max="226" width="12" style="228"/>
+    <col min="227" max="227" width="12" style="229"/>
+    <col min="228" max="228" width="12" style="230"/>
+    <col min="229" max="229" width="12" style="231"/>
+    <col min="230" max="230" width="12" style="232"/>
+    <col min="231" max="231" width="12" style="233"/>
+    <col min="232" max="232" width="12" style="234"/>
+    <col min="233" max="233" width="12" style="235"/>
+    <col min="234" max="234" width="12" style="236"/>
+    <col min="235" max="235" width="12" style="237"/>
+    <col min="236" max="236" width="12" style="238"/>
+    <col min="237" max="237" width="12" style="239"/>
+    <col min="238" max="238" width="12" style="240"/>
+    <col min="239" max="239" width="12" style="241"/>
+    <col min="240" max="240" width="12" style="242"/>
+    <col min="241" max="241" width="12" style="243"/>
+    <col min="242" max="242" width="12" style="244"/>
+    <col min="243" max="243" width="12" style="245"/>
+    <col min="244" max="244" width="12" style="246"/>
+    <col min="245" max="245" width="12" style="247"/>
+    <col min="246" max="246" width="12" style="248"/>
+    <col min="247" max="247" width="12" style="249"/>
+    <col min="248" max="248" width="12" style="250"/>
+    <col min="249" max="249" width="12" style="251"/>
+    <col min="250" max="250" width="12" style="252"/>
+    <col min="251" max="251" width="12" style="253"/>
+    <col min="252" max="252" width="12" style="254"/>
+    <col min="253" max="253" width="12" style="255"/>
+    <col min="254" max="254" width="12" style="256"/>
+    <col min="255" max="255" width="12" style="257"/>
+    <col min="256" max="256" width="12" style="258"/>
+    <col min="257" max="257" width="12" style="259"/>
+    <col min="258" max="258" width="12" style="260"/>
+    <col min="259" max="259" width="12" style="261"/>
+    <col min="260" max="260" width="12" style="262"/>
+    <col min="261" max="261" width="12" style="263"/>
+    <col min="262" max="262" width="12" style="264"/>
+    <col min="263" max="263" width="12" style="265"/>
+    <col min="264" max="264" width="12" style="266"/>
+    <col min="265" max="265" width="12" style="267"/>
+    <col min="266" max="266" width="12" style="268"/>
+    <col min="267" max="267" width="12" style="269"/>
+    <col min="268" max="268" width="12" style="270"/>
+    <col min="269" max="269" width="12" style="271"/>
+    <col min="270" max="270" width="12" style="272"/>
+    <col min="271" max="271" width="12" style="273"/>
+    <col min="272" max="272" width="12" style="274"/>
+    <col min="273" max="273" width="12" style="275"/>
+    <col min="274" max="274" width="12" style="276"/>
+    <col min="275" max="275" width="12" style="277"/>
+    <col min="276" max="276" width="12" style="278"/>
+    <col min="277" max="277" width="12" style="279"/>
+    <col min="278" max="278" width="12" style="280"/>
+    <col min="279" max="279" width="12" style="281"/>
+    <col min="280" max="280" width="12" style="282"/>
+    <col min="281" max="281" width="12" style="283"/>
+    <col min="282" max="282" width="12" style="284"/>
+    <col min="283" max="283" width="12" style="285"/>
+    <col min="284" max="284" width="12" style="286"/>
+    <col min="285" max="285" width="12" style="287"/>
+    <col min="286" max="286" width="12" style="288"/>
+    <col min="287" max="287" width="12" style="289"/>
+    <col min="288" max="288" width="12" style="290"/>
+    <col min="289" max="289" width="12" style="291"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:287" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:289" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2750,7 +2866,7 @@
         <v>28</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>561</v>
+        <v>30</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>32</v>
@@ -2936,637 +3052,643 @@
         <v>152</v>
       </c>
       <c r="BZ1" s="1" t="s">
-        <v>30</v>
+        <v>154</v>
       </c>
       <c r="CA1" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="CB1" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="CC1" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="CD1" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="CE1" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CF1" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="CG1" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="CH1" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="CI1" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="CJ1" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="CK1" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="CL1" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="CM1" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="CN1" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="CO1" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="CP1" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="CQ1" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="CR1" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="CS1" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="CT1" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="CU1" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="CV1" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="CW1" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="CX1" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="CY1" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="CZ1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="DA1" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="DB1" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="DC1" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="DD1" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="DE1" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="DF1" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="DG1" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="DH1" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="DI1" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="DJ1" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="DK1" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="DL1" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="DM1" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="DN1" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="DO1" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="DP1" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="DQ1" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="DR1" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="DS1" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="DT1" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="DU1" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="DV1" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="DW1" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="DX1" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="DY1" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="DZ1" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="EA1" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="EB1" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="EC1" s="1" t="s">
-        <v>263</v>
+        <v>256</v>
+      </c>
+      <c r="DZ1" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="EA1" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="EB1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="EC1" s="2" t="s">
+        <v>264</v>
       </c>
       <c r="ED1" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="EE1" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="EF1" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="EG1" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="EH1" s="2" t="s">
-        <v>273</v>
+        <v>268</v>
+      </c>
+      <c r="EF1" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="EG1" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="EH1" s="1" t="s">
+        <v>274</v>
       </c>
       <c r="EI1" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="EJ1" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="EK1" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="EL1" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="EM1" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="EN1" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="EO1" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
+      </c>
+      <c r="EO1" s="2" t="s">
+        <v>288</v>
       </c>
       <c r="EP1" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="EQ1" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="ER1" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
+      </c>
+      <c r="ER1" s="1" t="s">
+        <v>294</v>
       </c>
       <c r="ES1" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="ET1" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="EU1" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="EV1" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="EW1" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
+      </c>
+      <c r="EW1" s="2" t="s">
+        <v>304</v>
       </c>
       <c r="EX1" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="EY1" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="EZ1" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="FA1" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="FB1" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="FC1" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
+      </c>
+      <c r="FC1" s="1" t="s">
+        <v>316</v>
       </c>
       <c r="FD1" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="FE1" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="FF1" s="2" t="s">
-        <v>321</v>
+        <v>318</v>
+      </c>
+      <c r="FE1" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="FF1" s="1" t="s">
+        <v>322</v>
       </c>
       <c r="FG1" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="FH1" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="FI1" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="FJ1" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="FK1" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="FL1" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="FM1" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="FN1" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="FO1" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="FP1" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="FQ1" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="FR1" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="FS1" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
+      </c>
+      <c r="FS1" s="2" t="s">
+        <v>348</v>
       </c>
       <c r="FT1" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="FU1" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="FV1" s="2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="FW1" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="FX1" s="1" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="FY1" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="FZ1" s="1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="GA1" s="1" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="GB1" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="GC1" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="GD1" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
+      </c>
+      <c r="GD1" s="2" t="s">
+        <v>370</v>
       </c>
       <c r="GE1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="GF1" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="GG1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="GH1" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="GI1" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="GJ1" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="GK1" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="GL1" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="GM1" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="GN1" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="GO1" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="GP1" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="GQ1" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="GR1" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="GS1" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="GT1" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="GU1" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="GV1" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="GW1" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="GX1" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="GY1" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="GZ1" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="HA1" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="HB1" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="HC1" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="HD1" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="HE1" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="HF1" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="HG1" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="HH1" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="HI1" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="HJ1" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="HK1" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="HL1" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="HM1" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="HN1" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="HO1" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="HP1" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="HQ1" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="HR1" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="HS1" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="HT1" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="HU1" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="HV1" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="HW1" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="HX1" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="HY1" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="HZ1" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="IA1" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="IB1" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="IC1" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="ID1" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="IE1" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="IF1" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="IG1" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="IH1" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="II1" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="IJ1" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="IK1" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="IL1" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="IM1" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="IN1" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="IO1" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="IP1" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="IQ1" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="IR1" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="IS1" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="IT1" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="IU1" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="IV1" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="IW1" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="IX1" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="IY1" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="IZ1" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="JA1" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="JB1" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="JC1" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="JD1" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="JE1" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="JF1" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="JG1" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="JH1" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="JI1" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="JJ1" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="JK1" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="JL1" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="JM1" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="JN1" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="JO1" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="JP1" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="JQ1" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="JR1" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="JS1" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="JT1" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="JU1" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="JV1" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="JW1" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="JX1" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="JY1" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="JZ1" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="KA1" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="KB1" s="1" t="s">
         <v>562</v>
       </c>
-      <c r="GF1" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="GG1" s="2" t="s">
-        <v>563</v>
-      </c>
-      <c r="GH1" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="GI1" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="GJ1" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="GK1" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="GL1" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="GM1" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="GN1" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="GO1" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="GP1" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="GQ1" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="GR1" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="GS1" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="GT1" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="GU1" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="GV1" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="GW1" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="GX1" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="GY1" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="GZ1" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="HA1" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="HB1" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="HC1" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="HD1" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="HE1" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="HF1" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="HG1" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="HH1" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="HI1" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="HJ1" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="HK1" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="HL1" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="HM1" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="HN1" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="HO1" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="HP1" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="HQ1" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="HR1" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="HS1" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="HT1" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="HU1" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="HV1" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="HW1" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="HX1" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="HY1" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="HZ1" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="IA1" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="IB1" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="IC1" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="ID1" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="IE1" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="IF1" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="IG1" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="IH1" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="II1" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="IJ1" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="IK1" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="IL1" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="IM1" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="IN1" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="IO1" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="IP1" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="IQ1" s="2" t="s">
+      <c r="KC1" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="IR1" s="1" t="s">
-        <v>565</v>
-      </c>
-      <c r="IS1" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="IT1" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="IU1" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="IV1" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="IW1" s="2" t="s">
-        <v>507</v>
-      </c>
-      <c r="IX1" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="IY1" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="IZ1" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="JA1" s="1" t="s">
-        <v>566</v>
-      </c>
-      <c r="JB1" s="1" t="s">
-        <v>516</v>
-      </c>
-      <c r="JC1" s="2" t="s">
-        <v>518</v>
-      </c>
-      <c r="JD1" s="2" t="s">
-        <v>520</v>
-      </c>
-      <c r="JE1" s="2" t="s">
-        <v>522</v>
-      </c>
-      <c r="JF1" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="JG1" s="1" t="s">
-        <v>567</v>
-      </c>
-      <c r="JH1" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="JI1" s="1" t="s">
-        <v>569</v>
-      </c>
-      <c r="JJ1" s="1" t="s">
-        <v>570</v>
-      </c>
-      <c r="JK1" s="1" t="s">
-        <v>571</v>
-      </c>
-      <c r="JL1" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="JM1" s="1" t="s">
-        <v>573</v>
-      </c>
-      <c r="JN1" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="JO1" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="JP1" s="1" t="s">
-        <v>537</v>
-      </c>
-      <c r="JQ1" s="1" t="s">
-        <v>539</v>
-      </c>
-      <c r="JR1" s="1" t="s">
-        <v>541</v>
-      </c>
-      <c r="JS1" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="JT1" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="JU1" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="JV1" s="1" t="s">
-        <v>549</v>
-      </c>
-      <c r="JW1" s="1" t="s">
-        <v>551</v>
-      </c>
-      <c r="JX1" s="1" t="s">
-        <v>553</v>
-      </c>
-      <c r="JY1" s="1" t="s">
-        <v>555</v>
-      </c>
-      <c r="JZ1" s="1" t="s">
-        <v>557</v>
-      </c>
-      <c r="KA1" s="1" t="s">
-        <v>559</v>
-      </c>
     </row>
-    <row r="2" spans="1:287" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:289" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -3799,638 +3921,644 @@
         <v>153</v>
       </c>
       <c r="BZ2" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="CA2" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="CB2" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="CC2" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="CD2" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="CE2" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="CF2" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="CG2" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="CH2" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="CI2" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="CJ2" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="CK2" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="CL2" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="CM2" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="CN2" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CO2" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="CP2" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CQ2" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="CR2" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="CS2" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="CT2" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="CU2" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="CV2" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="CW2" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="CX2" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="CY2" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="CZ2" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="DA2" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="DB2" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="DC2" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="DD2" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="DE2" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="DF2" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="DG2" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="DH2" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="DI2" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="DJ2" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="DK2" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="DL2" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="DM2" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="DN2" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="DO2" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="DP2" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="DQ2" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="DR2" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="DS2" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="DT2" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="DU2" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="DV2" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="DW2" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="DX2" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="DY2" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="DZ2" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="EA2" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="EB2" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="EC2" s="1" t="s">
-        <v>264</v>
+        <v>257</v>
+      </c>
+      <c r="DZ2" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="EA2" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="EB2" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="EC2" s="2" t="s">
+        <v>265</v>
       </c>
       <c r="ED2" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="EE2" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="EF2" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="EG2" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="EH2" s="2" t="s">
-        <v>274</v>
+        <v>269</v>
+      </c>
+      <c r="EF2" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="EG2" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="EH2" s="1" t="s">
+        <v>275</v>
       </c>
       <c r="EI2" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="EJ2" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="EK2" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="EL2" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="EM2" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="EN2" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="EO2" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
+      </c>
+      <c r="EO2" s="2" t="s">
+        <v>289</v>
       </c>
       <c r="EP2" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="EQ2" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="ER2" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
+      </c>
+      <c r="ER2" s="1" t="s">
+        <v>295</v>
       </c>
       <c r="ES2" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="ET2" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="EU2" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="EV2" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="EW2" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
+      </c>
+      <c r="EW2" s="2" t="s">
+        <v>305</v>
       </c>
       <c r="EX2" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="EY2" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="EZ2" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="FA2" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="FB2" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="FC2" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
+      </c>
+      <c r="FC2" s="1" t="s">
+        <v>317</v>
       </c>
       <c r="FD2" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="FE2" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="FF2" s="2" t="s">
-        <v>322</v>
+        <v>319</v>
+      </c>
+      <c r="FE2" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="FF2" s="1" t="s">
+        <v>323</v>
       </c>
       <c r="FG2" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="FH2" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="FI2" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="FJ2" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="FK2" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="FL2" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="FM2" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="FN2" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="FO2" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="FP2" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="FQ2" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="FR2" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="FS2" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
+      </c>
+      <c r="FS2" s="2" t="s">
+        <v>349</v>
       </c>
       <c r="FT2" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="FU2" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="FV2" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="FW2" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="FX2" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="FY2" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="FZ2" s="1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="GA2" s="1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="GB2" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="GC2" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="GD2" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
+      </c>
+      <c r="GD2" s="2" t="s">
+        <v>371</v>
       </c>
       <c r="GE2" s="2" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="GF2" s="2" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="GG2" s="2" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="GH2" s="2" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="GI2" s="2" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="GJ2" s="1" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="GK2" s="1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="GL2" s="1" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="GM2" s="1" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="GN2" s="1" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="GO2" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="GP2" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="GQ2" s="1" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="GR2" s="1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="GS2" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="GT2" s="1" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="GU2" s="1" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="GV2" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="GW2" s="1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="GX2" s="1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="GY2" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="GZ2" s="2" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="HA2" s="2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="HB2" s="2" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="HC2" s="2" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="HD2" s="2" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="HE2" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="HF2" s="2" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="HG2" s="1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="HH2" s="2" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="HI2" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="HJ2" s="2" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="HK2" s="2" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="HL2" s="1" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="HM2" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="HN2" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="HO2" s="2" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="HP2" s="2" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="HQ2" s="2" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="HR2" s="2" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="HS2" s="1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="HT2" s="1" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="HU2" s="1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="HV2" s="1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="HW2" s="1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="HX2" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="HY2" s="1" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="HZ2" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="IA2" s="1" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="IB2" s="1" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="IC2" s="1" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="ID2" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="IE2" s="1" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="IF2" s="1" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="IG2" s="1" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="IH2" s="1" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="II2" s="1" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="IJ2" s="1" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="IK2" s="1" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="IL2" s="1" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="IM2" s="1" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="IN2" s="1" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="IO2" s="1" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="IP2" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="IQ2" s="2" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="IR2" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="IS2" s="1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="IT2" s="1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="IU2" s="2" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="IV2" s="1" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="IW2" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="IX2" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="IY2" s="2" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="IZ2" s="1" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="JA2" s="1" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="JB2" s="1" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="JC2" s="2" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="JD2" s="2" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="JE2" s="2" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="JF2" s="1" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="JG2" s="1" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="JH2" s="1" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="JI2" s="1" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="JJ2" s="1" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="JK2" s="1" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="JL2" s="1" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="JM2" s="1" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="JN2" s="1" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="JO2" s="1" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="JP2" s="1" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="JQ2" s="1" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="JR2" s="1" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="JS2" s="1" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="JT2" s="1" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="JU2" s="1" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="JV2" s="1" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="JW2" s="1" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="JX2" s="1" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="JY2" s="1" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="JZ2" s="1" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="KA2" s="1" t="s">
-        <v>560</v>
+        <v>561</v>
+      </c>
+      <c r="KB2" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="KC2" s="1" t="s">
+        <v>565</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SKU validation done to deploy in test server 11-16-2021
</commit_message>
<xml_diff>
--- a/files/temporaryTemplates/TempOrderHoneywell.xlsx
+++ b/files/temporaryTemplates/TempOrderHoneywell.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Reports\conversionToolBack\files\temporaryTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB4B36F1-C7D8-4395-A7A4-2693B99546E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4347B9C7-EE0F-4284-A114-9A97EB4E67CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shipment Order Details" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <author>FLUX</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -39,7 +39,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -53,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -67,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -81,7 +81,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DL1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="DN1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -95,7 +95,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DM1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="DO1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -109,7 +109,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DN1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="DP1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -123,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EH1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="EJ1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -137,7 +137,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EK1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="EM1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -2523,201 +2523,201 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" style="3"/>
-    <col min="2" max="2" width="12" style="4"/>
-    <col min="3" max="3" width="12" style="5"/>
-    <col min="4" max="4" width="12" style="6"/>
-    <col min="5" max="5" width="12" style="7"/>
-    <col min="6" max="6" width="12" style="8"/>
-    <col min="7" max="7" width="12" style="9"/>
-    <col min="8" max="8" width="12" style="10"/>
-    <col min="9" max="9" width="12" style="11"/>
-    <col min="10" max="10" width="12" style="12"/>
-    <col min="11" max="11" width="12" style="13"/>
-    <col min="12" max="12" width="12" style="14"/>
-    <col min="13" max="13" width="12" style="15"/>
-    <col min="14" max="14" width="12" style="16"/>
-    <col min="15" max="15" width="12" style="17"/>
-    <col min="16" max="16" width="12" style="18"/>
-    <col min="17" max="17" width="12" style="19"/>
-    <col min="18" max="18" width="12" style="20"/>
-    <col min="19" max="19" width="12" style="21"/>
-    <col min="20" max="20" width="12" style="22"/>
-    <col min="21" max="21" width="12" style="23"/>
-    <col min="22" max="22" width="12" style="24"/>
-    <col min="23" max="23" width="12" style="25"/>
-    <col min="24" max="24" width="12" style="26"/>
-    <col min="25" max="25" width="12" style="27"/>
-    <col min="26" max="26" width="12" style="28"/>
-    <col min="27" max="27" width="12" style="29"/>
-    <col min="28" max="28" width="12" style="30"/>
-    <col min="29" max="29" width="12" style="31"/>
-    <col min="30" max="30" width="12" style="32"/>
-    <col min="31" max="31" width="12" style="33"/>
-    <col min="32" max="32" width="12" style="34"/>
-    <col min="33" max="33" width="12" style="35"/>
-    <col min="34" max="34" width="12" style="36"/>
-    <col min="35" max="35" width="12" style="37"/>
-    <col min="36" max="36" width="12" style="38"/>
-    <col min="37" max="37" width="12" style="39"/>
-    <col min="38" max="38" width="12" style="40"/>
-    <col min="39" max="39" width="12" style="41"/>
-    <col min="40" max="40" width="12" style="42"/>
-    <col min="41" max="41" width="12" style="43"/>
-    <col min="42" max="42" width="12" style="44"/>
-    <col min="43" max="43" width="12" style="45"/>
-    <col min="44" max="44" width="12" style="46"/>
-    <col min="45" max="45" width="12" style="47"/>
-    <col min="46" max="46" width="12" style="48"/>
-    <col min="47" max="47" width="12" style="49"/>
-    <col min="48" max="48" width="12" style="50"/>
-    <col min="49" max="49" width="12" style="51"/>
-    <col min="50" max="50" width="12" style="52"/>
-    <col min="51" max="51" width="12" style="53"/>
-    <col min="52" max="52" width="12" style="54"/>
-    <col min="53" max="53" width="12" style="55"/>
-    <col min="54" max="54" width="12" style="56"/>
-    <col min="55" max="55" width="12" style="57"/>
-    <col min="56" max="56" width="12" style="58"/>
-    <col min="57" max="57" width="12" style="59"/>
-    <col min="58" max="58" width="12" style="60"/>
-    <col min="59" max="59" width="12" style="61"/>
-    <col min="60" max="60" width="12" style="62"/>
-    <col min="61" max="61" width="12" style="63"/>
-    <col min="62" max="62" width="12" style="64"/>
-    <col min="63" max="63" width="12" style="65"/>
-    <col min="64" max="64" width="12" style="66"/>
-    <col min="65" max="65" width="12" style="67"/>
-    <col min="66" max="66" width="12" style="68"/>
-    <col min="67" max="67" width="12" style="69"/>
-    <col min="68" max="68" width="12" style="70"/>
-    <col min="69" max="69" width="12" style="71"/>
-    <col min="70" max="70" width="12" style="72"/>
-    <col min="71" max="71" width="12" style="73"/>
-    <col min="72" max="72" width="12" style="74"/>
-    <col min="73" max="73" width="12" style="75"/>
-    <col min="74" max="74" width="12" style="76"/>
-    <col min="75" max="75" width="12" style="77"/>
-    <col min="76" max="76" width="12" style="78"/>
-    <col min="77" max="77" width="12" style="79"/>
-    <col min="78" max="78" width="12" style="80"/>
-    <col min="79" max="79" width="12" style="81"/>
-    <col min="80" max="80" width="12" style="82"/>
-    <col min="81" max="81" width="12" style="83"/>
-    <col min="82" max="82" width="12" style="84"/>
-    <col min="83" max="83" width="12" style="85"/>
-    <col min="84" max="84" width="12" style="86"/>
-    <col min="85" max="85" width="12" style="87"/>
-    <col min="86" max="86" width="12" style="88"/>
-    <col min="87" max="87" width="12" style="89"/>
-    <col min="88" max="88" width="12" style="90"/>
-    <col min="89" max="89" width="12" style="91"/>
-    <col min="90" max="90" width="12" style="92"/>
-    <col min="91" max="91" width="12" style="93"/>
-    <col min="92" max="92" width="12" style="94"/>
-    <col min="93" max="93" width="12" style="95"/>
-    <col min="94" max="94" width="12" style="96"/>
-    <col min="95" max="95" width="12" style="97"/>
-    <col min="96" max="96" width="12" style="98"/>
-    <col min="97" max="97" width="12" style="99"/>
-    <col min="98" max="98" width="12" style="100"/>
-    <col min="99" max="99" width="12" style="101"/>
-    <col min="100" max="100" width="12" style="102"/>
-    <col min="101" max="101" width="12" style="103"/>
-    <col min="102" max="102" width="12" style="104"/>
-    <col min="103" max="103" width="12" style="105"/>
-    <col min="104" max="104" width="12" style="106"/>
-    <col min="105" max="105" width="12" style="107"/>
-    <col min="106" max="106" width="12" style="108"/>
-    <col min="107" max="107" width="12" style="109"/>
-    <col min="108" max="108" width="12" style="110"/>
-    <col min="109" max="109" width="12" style="111"/>
-    <col min="110" max="110" width="12" style="112"/>
-    <col min="111" max="111" width="12" style="113"/>
-    <col min="112" max="112" width="12" style="114"/>
-    <col min="113" max="113" width="12" style="115"/>
-    <col min="114" max="114" width="12" style="116"/>
-    <col min="115" max="115" width="12" style="117"/>
-    <col min="116" max="116" width="12" style="118"/>
-    <col min="117" max="117" width="12" style="119"/>
-    <col min="118" max="118" width="12" style="120"/>
-    <col min="119" max="119" width="12" style="121"/>
-    <col min="120" max="120" width="12" style="122"/>
-    <col min="121" max="121" width="12" style="123"/>
-    <col min="122" max="122" width="12" style="124"/>
-    <col min="123" max="123" width="12" style="125"/>
-    <col min="124" max="124" width="12" style="126"/>
-    <col min="125" max="125" width="12" style="127"/>
-    <col min="126" max="126" width="12" style="128"/>
-    <col min="127" max="127" width="12" style="129"/>
-    <col min="128" max="128" width="12" style="130"/>
-    <col min="129" max="129" width="12" style="131"/>
-    <col min="130" max="130" width="12" style="132"/>
-    <col min="131" max="131" width="12" style="133"/>
-    <col min="132" max="132" width="12" style="134"/>
-    <col min="133" max="133" width="12" style="135"/>
-    <col min="134" max="134" width="12" style="136"/>
-    <col min="135" max="135" width="12" style="137"/>
-    <col min="136" max="136" width="12" style="138"/>
-    <col min="137" max="137" width="12" style="139"/>
-    <col min="138" max="138" width="12" style="140"/>
-    <col min="139" max="139" width="12" style="141"/>
-    <col min="140" max="140" width="12" style="142"/>
-    <col min="141" max="141" width="12" style="143"/>
-    <col min="142" max="142" width="12" style="144"/>
-    <col min="143" max="143" width="12" style="145"/>
-    <col min="144" max="144" width="12" style="146"/>
-    <col min="145" max="145" width="12" style="147"/>
-    <col min="146" max="146" width="12" style="148"/>
-    <col min="147" max="147" width="12" style="149"/>
-    <col min="148" max="148" width="12" style="150"/>
-    <col min="149" max="149" width="12" style="151"/>
-    <col min="150" max="150" width="12" style="152"/>
-    <col min="151" max="151" width="12" style="153"/>
-    <col min="152" max="152" width="12" style="154"/>
-    <col min="153" max="153" width="12" style="155"/>
-    <col min="154" max="154" width="12" style="156"/>
-    <col min="155" max="155" width="12" style="157"/>
-    <col min="156" max="156" width="12" style="158"/>
-    <col min="157" max="157" width="12" style="159"/>
-    <col min="158" max="158" width="12" style="160"/>
-    <col min="159" max="159" width="12" style="161"/>
-    <col min="160" max="160" width="12" style="162"/>
-    <col min="161" max="161" width="12" style="163"/>
-    <col min="162" max="162" width="12" style="164"/>
-    <col min="163" max="163" width="12" style="165"/>
-    <col min="164" max="164" width="12" style="166"/>
-    <col min="165" max="165" width="12" style="167"/>
-    <col min="166" max="166" width="12" style="168"/>
-    <col min="167" max="167" width="12" style="169"/>
-    <col min="168" max="168" width="12" style="170"/>
-    <col min="169" max="169" width="12" style="171"/>
-    <col min="170" max="170" width="12" style="172"/>
-    <col min="171" max="171" width="12" style="173"/>
-    <col min="172" max="172" width="12" style="174"/>
-    <col min="173" max="173" width="12" style="175"/>
-    <col min="174" max="174" width="12" style="176"/>
-    <col min="175" max="175" width="12" style="177"/>
-    <col min="176" max="176" width="12" style="178"/>
-    <col min="177" max="177" width="12" style="179"/>
-    <col min="178" max="178" width="12" style="180"/>
-    <col min="179" max="179" width="12" style="181"/>
-    <col min="180" max="180" width="12" style="182"/>
-    <col min="181" max="181" width="12" style="183"/>
-    <col min="182" max="182" width="12" style="184"/>
-    <col min="183" max="183" width="12" style="185"/>
-    <col min="184" max="184" width="12" style="186"/>
-    <col min="185" max="185" width="12" style="187"/>
-    <col min="186" max="186" width="12" style="188"/>
-    <col min="187" max="187" width="12" style="189"/>
-    <col min="188" max="188" width="12" style="190"/>
-    <col min="189" max="189" width="12" style="191"/>
-    <col min="190" max="190" width="12" style="192"/>
+    <col min="1" max="1" width="14.140625" style="190" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="192" customWidth="1"/>
+    <col min="3" max="3" width="12" style="3"/>
+    <col min="4" max="4" width="12" style="4"/>
+    <col min="5" max="5" width="12" style="5"/>
+    <col min="6" max="6" width="12" style="6"/>
+    <col min="7" max="7" width="12" style="7"/>
+    <col min="8" max="8" width="12" style="8"/>
+    <col min="9" max="9" width="12" style="9"/>
+    <col min="10" max="10" width="12" style="10"/>
+    <col min="11" max="11" width="12" style="11"/>
+    <col min="12" max="12" width="12" style="12"/>
+    <col min="13" max="13" width="12" style="13"/>
+    <col min="14" max="14" width="12" style="14"/>
+    <col min="15" max="15" width="12" style="15"/>
+    <col min="16" max="16" width="12" style="16"/>
+    <col min="17" max="17" width="12" style="17"/>
+    <col min="18" max="18" width="12" style="18"/>
+    <col min="19" max="19" width="12" style="19"/>
+    <col min="20" max="20" width="12" style="20"/>
+    <col min="21" max="21" width="12" style="21"/>
+    <col min="22" max="22" width="12" style="22"/>
+    <col min="23" max="23" width="12" style="23"/>
+    <col min="24" max="24" width="12" style="24"/>
+    <col min="25" max="25" width="12" style="25"/>
+    <col min="26" max="26" width="12" style="26"/>
+    <col min="27" max="27" width="12" style="27"/>
+    <col min="28" max="28" width="12" style="28"/>
+    <col min="29" max="29" width="12" style="29"/>
+    <col min="30" max="30" width="12" style="30"/>
+    <col min="31" max="31" width="12" style="31"/>
+    <col min="32" max="32" width="12" style="32"/>
+    <col min="33" max="33" width="12" style="33"/>
+    <col min="34" max="34" width="12" style="34"/>
+    <col min="35" max="35" width="12" style="35"/>
+    <col min="36" max="36" width="12" style="36"/>
+    <col min="37" max="37" width="12" style="37"/>
+    <col min="38" max="38" width="12" style="38"/>
+    <col min="39" max="39" width="12" style="39"/>
+    <col min="40" max="40" width="12" style="40"/>
+    <col min="41" max="41" width="12" style="41"/>
+    <col min="42" max="42" width="12" style="42"/>
+    <col min="43" max="43" width="12" style="43"/>
+    <col min="44" max="44" width="12" style="44"/>
+    <col min="45" max="45" width="12" style="45"/>
+    <col min="46" max="46" width="12" style="46"/>
+    <col min="47" max="47" width="12" style="47"/>
+    <col min="48" max="48" width="12" style="48"/>
+    <col min="49" max="49" width="12" style="49"/>
+    <col min="50" max="50" width="12" style="50"/>
+    <col min="51" max="51" width="12" style="51"/>
+    <col min="52" max="52" width="12" style="52"/>
+    <col min="53" max="53" width="12" style="53"/>
+    <col min="54" max="54" width="12" style="54"/>
+    <col min="55" max="55" width="12" style="55"/>
+    <col min="56" max="56" width="12" style="56"/>
+    <col min="57" max="57" width="12" style="57"/>
+    <col min="58" max="58" width="12" style="58"/>
+    <col min="59" max="59" width="12" style="59"/>
+    <col min="60" max="60" width="12" style="60"/>
+    <col min="61" max="61" width="12" style="61"/>
+    <col min="62" max="62" width="12" style="62"/>
+    <col min="63" max="63" width="12" style="63"/>
+    <col min="64" max="64" width="12" style="64"/>
+    <col min="65" max="65" width="12" style="65"/>
+    <col min="66" max="66" width="12" style="66"/>
+    <col min="67" max="67" width="12" style="67"/>
+    <col min="68" max="68" width="12" style="68"/>
+    <col min="69" max="69" width="12" style="69"/>
+    <col min="70" max="70" width="12" style="70"/>
+    <col min="71" max="71" width="12" style="71"/>
+    <col min="72" max="72" width="12" style="72"/>
+    <col min="73" max="73" width="12" style="73"/>
+    <col min="74" max="74" width="12" style="74"/>
+    <col min="75" max="75" width="12" style="75"/>
+    <col min="76" max="76" width="12" style="76"/>
+    <col min="77" max="77" width="12" style="77"/>
+    <col min="78" max="78" width="12" style="78"/>
+    <col min="79" max="79" width="12" style="79"/>
+    <col min="80" max="80" width="12" style="80"/>
+    <col min="81" max="81" width="12" style="81"/>
+    <col min="82" max="82" width="12" style="82"/>
+    <col min="83" max="83" width="12" style="83"/>
+    <col min="84" max="84" width="12" style="84"/>
+    <col min="85" max="85" width="12" style="85"/>
+    <col min="86" max="86" width="12" style="86"/>
+    <col min="87" max="87" width="12" style="87"/>
+    <col min="88" max="88" width="12" style="88"/>
+    <col min="89" max="89" width="12" style="89"/>
+    <col min="90" max="90" width="12" style="90"/>
+    <col min="91" max="91" width="12" style="91"/>
+    <col min="92" max="92" width="12" style="92"/>
+    <col min="93" max="93" width="12" style="93"/>
+    <col min="94" max="94" width="12" style="94"/>
+    <col min="95" max="95" width="12" style="95"/>
+    <col min="96" max="96" width="12" style="96"/>
+    <col min="97" max="97" width="12" style="97"/>
+    <col min="98" max="98" width="12" style="98"/>
+    <col min="99" max="99" width="12" style="99"/>
+    <col min="100" max="100" width="12" style="100"/>
+    <col min="101" max="101" width="12" style="101"/>
+    <col min="102" max="102" width="12" style="102"/>
+    <col min="103" max="103" width="12" style="103"/>
+    <col min="104" max="104" width="12" style="104"/>
+    <col min="105" max="105" width="12" style="105"/>
+    <col min="106" max="106" width="12" style="106"/>
+    <col min="107" max="107" width="12" style="107"/>
+    <col min="108" max="108" width="12" style="108"/>
+    <col min="109" max="109" width="12" style="109"/>
+    <col min="110" max="110" width="12" style="110"/>
+    <col min="111" max="111" width="12" style="111"/>
+    <col min="112" max="112" width="12" style="112"/>
+    <col min="113" max="113" width="12" style="113"/>
+    <col min="114" max="114" width="12" style="114"/>
+    <col min="115" max="115" width="12" style="115"/>
+    <col min="116" max="116" width="12" style="116"/>
+    <col min="117" max="117" width="12" style="117"/>
+    <col min="118" max="118" width="12" style="118"/>
+    <col min="119" max="119" width="12" style="119"/>
+    <col min="120" max="120" width="12" style="120"/>
+    <col min="121" max="121" width="12" style="121"/>
+    <col min="122" max="122" width="12" style="122"/>
+    <col min="123" max="123" width="12" style="123"/>
+    <col min="124" max="124" width="12" style="124"/>
+    <col min="125" max="125" width="12" style="125"/>
+    <col min="126" max="126" width="12" style="126"/>
+    <col min="127" max="127" width="12" style="127"/>
+    <col min="128" max="128" width="12" style="128"/>
+    <col min="129" max="129" width="12" style="129"/>
+    <col min="130" max="130" width="12" style="130"/>
+    <col min="131" max="131" width="12" style="131"/>
+    <col min="132" max="132" width="12" style="132"/>
+    <col min="133" max="133" width="12" style="133"/>
+    <col min="134" max="134" width="12" style="134"/>
+    <col min="135" max="135" width="12" style="135"/>
+    <col min="136" max="136" width="12" style="136"/>
+    <col min="137" max="137" width="12" style="137"/>
+    <col min="138" max="138" width="12" style="138"/>
+    <col min="139" max="139" width="12" style="139"/>
+    <col min="140" max="140" width="12" style="140"/>
+    <col min="141" max="141" width="12" style="141"/>
+    <col min="142" max="142" width="12" style="142"/>
+    <col min="143" max="143" width="12" style="143"/>
+    <col min="144" max="144" width="12" style="144"/>
+    <col min="145" max="145" width="12" style="145"/>
+    <col min="146" max="146" width="12" style="146"/>
+    <col min="147" max="147" width="12" style="147"/>
+    <col min="148" max="148" width="12" style="148"/>
+    <col min="149" max="149" width="12" style="149"/>
+    <col min="150" max="150" width="12" style="150"/>
+    <col min="151" max="151" width="12" style="151"/>
+    <col min="152" max="152" width="12" style="152"/>
+    <col min="153" max="153" width="12" style="153"/>
+    <col min="154" max="154" width="12" style="154"/>
+    <col min="155" max="155" width="12" style="155"/>
+    <col min="156" max="156" width="12" style="156"/>
+    <col min="157" max="157" width="12" style="157"/>
+    <col min="158" max="158" width="12" style="158"/>
+    <col min="159" max="159" width="12" style="159"/>
+    <col min="160" max="160" width="12" style="160"/>
+    <col min="161" max="161" width="12" style="161"/>
+    <col min="162" max="162" width="12" style="162"/>
+    <col min="163" max="163" width="15.140625" style="163" bestFit="1" customWidth="1"/>
+    <col min="164" max="164" width="12" style="164"/>
+    <col min="165" max="165" width="12" style="165"/>
+    <col min="166" max="166" width="12" style="166"/>
+    <col min="167" max="167" width="12" style="167"/>
+    <col min="168" max="168" width="12" style="168"/>
+    <col min="169" max="169" width="12" style="169"/>
+    <col min="170" max="170" width="12" style="170"/>
+    <col min="171" max="171" width="12" style="171"/>
+    <col min="172" max="172" width="12" style="172"/>
+    <col min="173" max="173" width="12" style="173"/>
+    <col min="174" max="174" width="12" style="174"/>
+    <col min="175" max="175" width="12" style="175"/>
+    <col min="176" max="176" width="12" style="176"/>
+    <col min="177" max="177" width="12" style="177"/>
+    <col min="178" max="178" width="12" style="178"/>
+    <col min="179" max="179" width="12" style="179"/>
+    <col min="180" max="180" width="12" style="180"/>
+    <col min="181" max="181" width="12" style="181"/>
+    <col min="182" max="182" width="12" style="182"/>
+    <col min="183" max="183" width="12" style="183"/>
+    <col min="184" max="184" width="12" style="184"/>
+    <col min="185" max="185" width="12" style="185"/>
+    <col min="186" max="186" width="12" style="186"/>
+    <col min="187" max="187" width="12" style="187"/>
+    <col min="188" max="188" width="12" style="188"/>
+    <col min="189" max="189" width="12" style="189"/>
+    <col min="190" max="190" width="12" style="191"/>
     <col min="191" max="191" width="12" style="193"/>
     <col min="192" max="192" width="12" style="194"/>
     <col min="193" max="193" width="12" style="195"/>
@@ -2821,574 +2821,574 @@
   <sheetData>
     <row r="1" spans="1:289" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BW1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CB1" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CC1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="CB1" s="1" t="s">
+      <c r="CD1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="CC1" s="1" t="s">
+      <c r="CE1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="CD1" s="1" t="s">
+      <c r="CF1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="CE1" s="1" t="s">
+      <c r="CG1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="CF1" s="1" t="s">
+      <c r="CH1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="CG1" s="1" t="s">
+      <c r="CI1" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="CH1" s="1" t="s">
+      <c r="CJ1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="CI1" s="1" t="s">
+      <c r="CK1" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="CJ1" s="1" t="s">
+      <c r="CL1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="CK1" s="1" t="s">
+      <c r="CM1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="CL1" s="1" t="s">
+      <c r="CN1" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="CM1" s="1" t="s">
+      <c r="CO1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="CN1" s="1" t="s">
+      <c r="CP1" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="CO1" s="1" t="s">
+      <c r="CQ1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="CP1" s="1" t="s">
+      <c r="CR1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="CQ1" s="1" t="s">
+      <c r="CS1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="CR1" s="1" t="s">
+      <c r="CT1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="CS1" s="1" t="s">
+      <c r="CU1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="CT1" s="1" t="s">
+      <c r="CV1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="CU1" s="1" t="s">
+      <c r="CW1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="CV1" s="1" t="s">
+      <c r="CX1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="CW1" s="1" t="s">
+      <c r="CY1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="CX1" s="1" t="s">
+      <c r="CZ1" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="CY1" s="1" t="s">
+      <c r="DA1" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="CZ1" s="1" t="s">
+      <c r="DB1" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="DA1" s="1" t="s">
+      <c r="DC1" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="DB1" s="1" t="s">
+      <c r="DD1" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="DC1" s="1" t="s">
+      <c r="DE1" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="DD1" s="1" t="s">
+      <c r="DF1" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="DE1" s="1" t="s">
+      <c r="DG1" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="DF1" s="1" t="s">
+      <c r="DH1" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="DG1" s="1" t="s">
+      <c r="DI1" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="DH1" s="1" t="s">
+      <c r="DJ1" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="DI1" s="1" t="s">
+      <c r="DK1" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="DJ1" s="1" t="s">
+      <c r="DL1" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="DK1" s="2" t="s">
+      <c r="DM1" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="DL1" s="1" t="s">
+      <c r="DN1" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="DM1" s="1" t="s">
+      <c r="DO1" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="DN1" s="1" t="s">
+      <c r="DP1" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="DO1" s="1" t="s">
+      <c r="DQ1" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="DP1" s="1" t="s">
+      <c r="DR1" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="DQ1" s="2" t="s">
+      <c r="DS1" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="DR1" s="1" t="s">
+      <c r="DT1" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="DS1" s="1" t="s">
+      <c r="DU1" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="DT1" s="2" t="s">
+      <c r="DV1" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="DU1" s="1" t="s">
+      <c r="DW1" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="DV1" s="1" t="s">
+      <c r="DX1" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="DW1" s="2" t="s">
+      <c r="DY1" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="DX1" s="2" t="s">
+      <c r="DZ1" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="DY1" s="2" t="s">
+      <c r="EA1" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="DZ1" s="1" t="s">
+      <c r="EB1" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="EA1" s="2" t="s">
+      <c r="EC1" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="EB1" s="1" t="s">
+      <c r="ED1" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="EC1" s="2" t="s">
+      <c r="EE1" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="ED1" s="2" t="s">
+      <c r="EF1" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="EE1" s="2" t="s">
+      <c r="EG1" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="EF1" s="1" t="s">
+      <c r="EH1" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="EG1" s="2" t="s">
+      <c r="EI1" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="EH1" s="1" t="s">
+      <c r="EJ1" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="EI1" s="1" t="s">
+      <c r="EK1" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="EJ1" s="1" t="s">
+      <c r="EL1" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="EK1" s="1" t="s">
+      <c r="EM1" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="EL1" s="1" t="s">
+      <c r="EN1" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="EM1" s="1" t="s">
+      <c r="EO1" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="EN1" s="1" t="s">
+      <c r="EP1" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="EO1" s="2" t="s">
+      <c r="EQ1" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="EP1" s="2" t="s">
+      <c r="ER1" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="EQ1" s="2" t="s">
+      <c r="ES1" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="ER1" s="1" t="s">
+      <c r="ET1" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="ES1" s="1" t="s">
+      <c r="EU1" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="ET1" s="1" t="s">
+      <c r="EV1" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="EU1" s="1" t="s">
+      <c r="EW1" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="EV1" s="1" t="s">
+      <c r="EX1" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="EW1" s="2" t="s">
+      <c r="EY1" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="EX1" s="2" t="s">
+      <c r="EZ1" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="EY1" s="2" t="s">
+      <c r="FA1" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="EZ1" s="2" t="s">
+      <c r="FB1" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="FA1" s="2" t="s">
+      <c r="FC1" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="FB1" s="2" t="s">
+      <c r="FD1" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="FC1" s="1" t="s">
+      <c r="FE1" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="FD1" s="1" t="s">
+      <c r="FF1" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="FE1" s="2" t="s">
+      <c r="FG1" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="FF1" s="1" t="s">
+      <c r="FH1" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="FG1" s="1" t="s">
+      <c r="FI1" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="FH1" s="1" t="s">
+      <c r="FJ1" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="FI1" s="1" t="s">
+      <c r="FK1" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="FJ1" s="1" t="s">
+      <c r="FL1" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="FK1" s="1" t="s">
+      <c r="FM1" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="FL1" s="1" t="s">
+      <c r="FN1" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="FM1" s="1" t="s">
+      <c r="FO1" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="FN1" s="1" t="s">
+      <c r="FP1" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="FO1" s="1" t="s">
+      <c r="FQ1" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="FP1" s="1" t="s">
+      <c r="FR1" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="FQ1" s="1" t="s">
+      <c r="FS1" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="FR1" s="1" t="s">
+      <c r="FT1" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="FS1" s="2" t="s">
+      <c r="FU1" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="FT1" s="1" t="s">
+      <c r="FV1" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="FU1" s="1" t="s">
+      <c r="FW1" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="FV1" s="2" t="s">
+      <c r="FX1" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="FW1" s="1" t="s">
+      <c r="FY1" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="FX1" s="1" t="s">
+      <c r="FZ1" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="FY1" s="1" t="s">
+      <c r="GA1" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="FZ1" s="1" t="s">
+      <c r="GB1" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="GA1" s="1" t="s">
+      <c r="GC1" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="GB1" s="1" t="s">
+      <c r="GD1" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="GC1" s="1" t="s">
+      <c r="GE1" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="GD1" s="2" t="s">
+      <c r="GF1" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="GE1" s="2" t="s">
+      <c r="GG1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="GF1" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="GG1" s="2" t="s">
+      <c r="GH1" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="GH1" s="2" t="s">
-        <v>376</v>
       </c>
       <c r="GI1" s="2" t="s">
         <v>378</v>
@@ -3690,574 +3690,574 @@
     </row>
     <row r="2" spans="1:289" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AK2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AJ2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AM2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AN2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AM2" s="1" t="s">
+      <c r="AO2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AN2" s="1" t="s">
+      <c r="AP2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AO2" s="1" t="s">
+      <c r="AQ2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AP2" s="1" t="s">
+      <c r="AR2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AQ2" s="1" t="s">
+      <c r="AS2" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="AR2" s="1" t="s">
+      <c r="AT2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AS2" s="1" t="s">
+      <c r="AU2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="AT2" s="1" t="s">
+      <c r="AV2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="AU2" s="1" t="s">
+      <c r="AW2" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="AV2" s="1" t="s">
+      <c r="AX2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="AW2" s="1" t="s">
+      <c r="AY2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AX2" s="1" t="s">
+      <c r="AZ2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AY2" s="1" t="s">
+      <c r="BA2" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="AZ2" s="1" t="s">
+      <c r="BB2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="BA2" s="1" t="s">
+      <c r="BC2" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="BB2" s="1" t="s">
+      <c r="BD2" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="BC2" s="1" t="s">
+      <c r="BE2" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="BD2" s="1" t="s">
+      <c r="BF2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="BE2" s="1" t="s">
+      <c r="BG2" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="BF2" s="1" t="s">
+      <c r="BH2" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="BG2" s="1" t="s">
+      <c r="BI2" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="BH2" s="1" t="s">
+      <c r="BJ2" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="BI2" s="1" t="s">
+      <c r="BK2" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="BJ2" s="1" t="s">
+      <c r="BL2" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="BK2" s="1" t="s">
+      <c r="BM2" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="BL2" s="1" t="s">
+      <c r="BN2" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="BM2" s="1" t="s">
+      <c r="BO2" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="BN2" s="1" t="s">
+      <c r="BP2" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="BO2" s="1" t="s">
+      <c r="BQ2" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="BP2" s="1" t="s">
+      <c r="BR2" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="BQ2" s="1" t="s">
+      <c r="BS2" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="BR2" s="1" t="s">
+      <c r="BT2" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="BS2" s="1" t="s">
+      <c r="BU2" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="BT2" s="1" t="s">
+      <c r="BV2" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="BU2" s="1" t="s">
+      <c r="BW2" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="BV2" s="1" t="s">
+      <c r="BX2" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="BW2" s="1" t="s">
+      <c r="BY2" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="BX2" s="1" t="s">
+      <c r="BZ2" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="BY2" s="1" t="s">
+      <c r="CA2" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="BZ2" s="1" t="s">
+      <c r="CB2" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="CA2" s="1" t="s">
+      <c r="CC2" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="CB2" s="1" t="s">
+      <c r="CD2" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="CC2" s="1" t="s">
+      <c r="CE2" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="CD2" s="1" t="s">
+      <c r="CF2" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="CE2" s="1" t="s">
+      <c r="CG2" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="CF2" s="1" t="s">
+      <c r="CH2" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="CG2" s="1" t="s">
+      <c r="CI2" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="CH2" s="1" t="s">
+      <c r="CJ2" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="CI2" s="1" t="s">
+      <c r="CK2" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="CJ2" s="1" t="s">
+      <c r="CL2" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="CK2" s="1" t="s">
+      <c r="CM2" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="CL2" s="1" t="s">
+      <c r="CN2" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="CM2" s="1" t="s">
+      <c r="CO2" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="CN2" s="1" t="s">
+      <c r="CP2" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="CO2" s="1" t="s">
+      <c r="CQ2" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="CP2" s="1" t="s">
+      <c r="CR2" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="CQ2" s="1" t="s">
+      <c r="CS2" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="CR2" s="1" t="s">
+      <c r="CT2" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="CS2" s="1" t="s">
+      <c r="CU2" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="CT2" s="1" t="s">
+      <c r="CV2" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="CU2" s="1" t="s">
+      <c r="CW2" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="CV2" s="1" t="s">
+      <c r="CX2" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="CW2" s="1" t="s">
+      <c r="CY2" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="CX2" s="1" t="s">
+      <c r="CZ2" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="CY2" s="1" t="s">
+      <c r="DA2" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="CZ2" s="1" t="s">
+      <c r="DB2" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="DA2" s="1" t="s">
+      <c r="DC2" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="DB2" s="1" t="s">
+      <c r="DD2" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="DC2" s="1" t="s">
+      <c r="DE2" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="DD2" s="1" t="s">
+      <c r="DF2" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="DE2" s="1" t="s">
+      <c r="DG2" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="DF2" s="1" t="s">
+      <c r="DH2" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="DG2" s="1" t="s">
+      <c r="DI2" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="DH2" s="1" t="s">
+      <c r="DJ2" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="DI2" s="1" t="s">
+      <c r="DK2" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="DJ2" s="1" t="s">
+      <c r="DL2" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="DK2" s="2" t="s">
+      <c r="DM2" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="DL2" s="1" t="s">
+      <c r="DN2" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="DM2" s="1" t="s">
+      <c r="DO2" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="DN2" s="1" t="s">
+      <c r="DP2" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="DO2" s="1" t="s">
+      <c r="DQ2" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="DP2" s="1" t="s">
+      <c r="DR2" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="DQ2" s="2" t="s">
+      <c r="DS2" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="DR2" s="1" t="s">
+      <c r="DT2" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="DS2" s="1" t="s">
+      <c r="DU2" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="DT2" s="2" t="s">
+      <c r="DV2" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="DU2" s="1" t="s">
+      <c r="DW2" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="DV2" s="1" t="s">
+      <c r="DX2" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="DW2" s="2" t="s">
+      <c r="DY2" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="DX2" s="2" t="s">
+      <c r="DZ2" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="DY2" s="2" t="s">
+      <c r="EA2" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="DZ2" s="1" t="s">
+      <c r="EB2" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="EA2" s="2" t="s">
+      <c r="EC2" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="EB2" s="1" t="s">
+      <c r="ED2" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="EC2" s="2" t="s">
+      <c r="EE2" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="ED2" s="2" t="s">
+      <c r="EF2" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="EE2" s="2" t="s">
+      <c r="EG2" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="EF2" s="1" t="s">
+      <c r="EH2" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="EG2" s="2" t="s">
+      <c r="EI2" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="EH2" s="1" t="s">
+      <c r="EJ2" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="EI2" s="1" t="s">
+      <c r="EK2" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="EJ2" s="1" t="s">
+      <c r="EL2" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="EK2" s="1" t="s">
+      <c r="EM2" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="EL2" s="1" t="s">
+      <c r="EN2" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="EM2" s="1" t="s">
+      <c r="EO2" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="EN2" s="1" t="s">
+      <c r="EP2" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="EO2" s="2" t="s">
+      <c r="EQ2" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="EP2" s="2" t="s">
+      <c r="ER2" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="EQ2" s="2" t="s">
+      <c r="ES2" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="ER2" s="1" t="s">
+      <c r="ET2" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="ES2" s="1" t="s">
+      <c r="EU2" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="ET2" s="1" t="s">
+      <c r="EV2" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="EU2" s="1" t="s">
+      <c r="EW2" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="EV2" s="1" t="s">
+      <c r="EX2" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="EW2" s="2" t="s">
+      <c r="EY2" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="EX2" s="2" t="s">
+      <c r="EZ2" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="EY2" s="2" t="s">
+      <c r="FA2" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="EZ2" s="2" t="s">
+      <c r="FB2" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="FA2" s="2" t="s">
+      <c r="FC2" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="FB2" s="2" t="s">
+      <c r="FD2" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="FC2" s="1" t="s">
+      <c r="FE2" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="FD2" s="1" t="s">
+      <c r="FF2" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="FE2" s="2" t="s">
+      <c r="FG2" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="FF2" s="1" t="s">
+      <c r="FH2" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="FG2" s="1" t="s">
+      <c r="FI2" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="FH2" s="1" t="s">
+      <c r="FJ2" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="FI2" s="1" t="s">
+      <c r="FK2" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="FJ2" s="1" t="s">
+      <c r="FL2" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="FK2" s="1" t="s">
+      <c r="FM2" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="FL2" s="1" t="s">
+      <c r="FN2" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="FM2" s="1" t="s">
+      <c r="FO2" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="FN2" s="1" t="s">
+      <c r="FP2" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="FO2" s="1" t="s">
+      <c r="FQ2" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="FP2" s="1" t="s">
+      <c r="FR2" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="FQ2" s="1" t="s">
+      <c r="FS2" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="FR2" s="1" t="s">
+      <c r="FT2" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="FS2" s="2" t="s">
+      <c r="FU2" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="FT2" s="1" t="s">
+      <c r="FV2" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="FU2" s="1" t="s">
+      <c r="FW2" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="FV2" s="2" t="s">
+      <c r="FX2" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="FW2" s="1" t="s">
+      <c r="FY2" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="FX2" s="1" t="s">
+      <c r="FZ2" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="FY2" s="1" t="s">
+      <c r="GA2" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="FZ2" s="1" t="s">
+      <c r="GB2" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="GA2" s="1" t="s">
+      <c r="GC2" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="GB2" s="1" t="s">
+      <c r="GD2" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="GC2" s="1" t="s">
+      <c r="GE2" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="GD2" s="2" t="s">
+      <c r="GF2" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="GE2" s="2" t="s">
+      <c r="GG2" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="GF2" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="GG2" s="2" t="s">
+      <c r="GH2" s="2" t="s">
         <v>375</v>
-      </c>
-      <c r="GH2" s="2" t="s">
-        <v>377</v>
       </c>
       <c r="GI2" s="2" t="s">
         <v>379</v>
@@ -4559,6 +4559,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>